<commit_message>
Changes in exception handling
</commit_message>
<xml_diff>
--- a/uploaded-files/success/HDFC Mid-Cap Opportunities Fund - 30 April 2025.xlsx
+++ b/uploaded-files/success/HDFC Mid-Cap Opportunities Fund - 30 April 2025.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7635"/>
   </bookViews>
@@ -52,541 +47,541 @@
   <definedNames>
     <definedName name="SheetKraft.IndicativeMode" hidden="1">TRUE</definedName>
     <definedName name="SheetKraftFormat">TRUE</definedName>
-    <definedName name="SheetKraftFormula1" hidden="1">_xll.Formula.SK('[1]Holding Positions'!$E$10,1)</definedName>
-    <definedName name="SheetKraftFormula10" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula100" hidden="1">_xll.Formula.SK([2]Stack!$AV$6,1)</definedName>
-    <definedName name="SheetKraftFormula101" hidden="1">_xll.Formula.SK([2]Stack!$AW$6,1)</definedName>
-    <definedName name="SheetKraftFormula102" hidden="1">_xll.Formula.SK([2]Stack!$AX$6,1)</definedName>
-    <definedName name="SheetKraftFormula104" hidden="1">_xll.Formula.SK([2]Stack!$BG$5,1)</definedName>
-    <definedName name="SheetKraftFormula105" hidden="1">_xll.Formula.SK([2]Stack!$CZ$6,1)</definedName>
-    <definedName name="SheetKraftFormula106" hidden="1">_xll.Formula.SK([2]Stack!$DI$5,1)</definedName>
-    <definedName name="SheetKraftFormula107" hidden="1">_xll.Formula.SK([2]Stack!$DH$5,1)</definedName>
-    <definedName name="SheetKraftFormula108" hidden="1">_xll.Formula.SK([3]Template_Formula!$A$3,1)</definedName>
-    <definedName name="SheetKraftFormula109" hidden="1">_xll.Formula.SK('[4]Asset Master'!$Y$7,1)</definedName>
-    <definedName name="SheetKraftFormula11" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula110" hidden="1">_xll.Formula.SK([2]Stack!$FC$5,1)</definedName>
-    <definedName name="SheetKraftFormula111" hidden="1">_xll.Formula.SK('[4]Asset Master'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula112" hidden="1">_xll.Formula.SK('[4]Asset Master'!$AI$10,1)</definedName>
-    <definedName name="SheetKraftFormula113" hidden="1">_xll.Formula.SK([2]Stack!$DB$5,1)</definedName>
-    <definedName name="SheetKraftFormula114" hidden="1">_xll.Formula.SK([2]Stack!$BF$5,1)</definedName>
-    <definedName name="SheetKraftFormula115" hidden="1">_xll.Formula.SK([2]Stack!$AZ$6,1)</definedName>
-    <definedName name="SheetKraftFormula116" hidden="1">_xll.Formula.SK([2]Stack!$AY$5,1)</definedName>
-    <definedName name="SheetKraftFormula117" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula118" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula119" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$R$5,1)</definedName>
-    <definedName name="SheetKraftFormula12" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula120" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AB$5,1)</definedName>
-    <definedName name="SheetKraftFormula121" hidden="1">_xll.Formula.SK([2]Stack!$BA$6,1)</definedName>
-    <definedName name="SheetKraftFormula123" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$I$4,)</definedName>
-    <definedName name="SheetKraftFormula124" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$L$4,)</definedName>
-    <definedName name="SheetKraftFormula125" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$S$4,)</definedName>
-    <definedName name="SheetKraftFormula126" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AP$4,)</definedName>
-    <definedName name="SheetKraftFormula127" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AQ$4,)</definedName>
-    <definedName name="SheetKraftFormula128" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AX$4,1)</definedName>
-    <definedName name="SheetKraftFormula129" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AZ$5,1)</definedName>
-    <definedName name="SheetKraftFormula13" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula130" hidden="1">_xll.Formula.SK([2]Stack!$BB$5,1)</definedName>
-    <definedName name="SheetKraftFormula131" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$B$4,1)</definedName>
-    <definedName name="SheetKraftFormula132" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$H$4,1)</definedName>
-    <definedName name="SheetKraftFormula133" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$J$5,1)</definedName>
-    <definedName name="SheetKraftFormula134" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BJ$4,1)</definedName>
-    <definedName name="SheetKraftFormula135" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$AC$4,1)</definedName>
-    <definedName name="SheetKraftFormula136" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$K$5,1)</definedName>
-    <definedName name="SheetKraftFormula137" hidden="1">_xll.Formula.SK([2]Stack!$DC$5,1)</definedName>
-    <definedName name="SheetKraftFormula138" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$AP$4,1)</definedName>
-    <definedName name="SheetKraftFormula139" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BA$4,1)</definedName>
-    <definedName name="SheetKraftFormula14" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula140" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$AI$4,1)</definedName>
-    <definedName name="SheetKraftFormula141" hidden="1">_xll.Formula.SK([3]Template_Formula!$A$10,1)</definedName>
-    <definedName name="SheetKraftFormula142" hidden="1">_xll.Formula.SK('[7]Notes Data'!$AH$9,1)</definedName>
-    <definedName name="SheetKraftFormula144" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BF$9,1)</definedName>
-    <definedName name="SheetKraftFormula145" hidden="1">_xll.Formula.SK('[7]Notes Data'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula146" hidden="1">_xll.Formula.SK('[7]Notes Data'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula147" hidden="1">_xll.Formula.SK([3]Template_Formula!$A$16,1)</definedName>
-    <definedName name="SheetKraftFormula148" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BI$9,1)</definedName>
-    <definedName name="SheetKraftFormula149" hidden="1">_xll.Formula.SK([3]Template_Formula!$A$15,1)</definedName>
-    <definedName name="SheetKraftFormula15" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula150" hidden="1">_xll.Formula.SK([3]Template_Formula!$O$9,1)</definedName>
-    <definedName name="SheetKraftFormula152" hidden="1">_xll.Formula.SK([8]Derivatives!$Y$10,1)</definedName>
-    <definedName name="SheetKraftFormula153" hidden="1">_xll.Formula.SK([8]Derivatives!$AA$11,1)</definedName>
-    <definedName name="SheetKraftFormula154" hidden="1">_xll.Formula.SK([8]Derivatives!$AB$11,1)</definedName>
-    <definedName name="SheetKraftFormula155" hidden="1">_xll.Formula.SK([3]Template_Formula!$O$14,1)</definedName>
-    <definedName name="SheetKraftFormula156" hidden="1">_xll.Formula.SK([8]Derivatives!$AF$10,1)</definedName>
-    <definedName name="SheetKraftFormula157" hidden="1">_xll.Formula.SK([8]Derivatives!$AH$10,1)</definedName>
-    <definedName name="SheetKraftFormula158" hidden="1">_xll.Formula.SK([8]Derivatives!$AI$11,1)</definedName>
-    <definedName name="SheetKraftFormula159" hidden="1">_xll.Formula.SK([8]Derivatives!$AI$10,)</definedName>
-    <definedName name="SheetKraftFormula16" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula160" hidden="1">_xll.Formula.SK([8]Derivatives!$AJ$10,)</definedName>
-    <definedName name="SheetKraftFormula161" hidden="1">_xll.Formula.SK([8]Derivatives!$AK$10,)</definedName>
-    <definedName name="SheetKraftFormula162" hidden="1">_xll.Formula.SK([8]Derivatives!$AO$10,1)</definedName>
-    <definedName name="SheetKraftFormula163" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$V$3,1)</definedName>
-    <definedName name="SheetKraftFormula164" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CK$9,1)</definedName>
-    <definedName name="SheetKraftFormula165" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CM$9,1)</definedName>
-    <definedName name="SheetKraftFormula167" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CO$9,)</definedName>
-    <definedName name="SheetKraftFormula168" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CN$9,)</definedName>
-    <definedName name="SheetKraftFormula169" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CQ$9,1)</definedName>
-    <definedName name="SheetKraftFormula17" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula170" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula171" hidden="1">_xll.Formula.SK('[7]Notes Data'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula172" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CR$9,1)</definedName>
-    <definedName name="SheetKraftFormula174" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CU$10,1)</definedName>
-    <definedName name="SheetKraftFormula175" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CV$10,1)</definedName>
-    <definedName name="SheetKraftFormula176" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CW$9,)</definedName>
-    <definedName name="SheetKraftFormula177" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CX$10,1)</definedName>
-    <definedName name="SheetKraftFormula178" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CK$10,1)</definedName>
-    <definedName name="SheetKraftFormula179" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CJ$10,1)</definedName>
-    <definedName name="SheetKraftFormula18" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula180" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula181" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula182" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula183" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula184" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula185" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula186" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula187" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula188" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula189" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula19" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula191" hidden="1">_xll.Formula.SK([9]Inputs!$Q$7,1)</definedName>
-    <definedName name="SheetKraftFormula192" hidden="1">_xll.Formula.SK('[10]Scheme Master'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula193" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula194" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula195" hidden="1">_xll.Formula.SK('[10]Scheme Master'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula196" hidden="1">_xll.Formula.SK('[10]Scheme Master'!$J$7,1)</definedName>
-    <definedName name="SheetKraftFormula197" hidden="1">_xll.Formula.SK('[11]Scheme Category'!$D$9,1)</definedName>
-    <definedName name="SheetKraftFormula198" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BE$9,1)</definedName>
-    <definedName name="SheetKraftFormula199" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BD$9,1)</definedName>
-    <definedName name="SheetKraftFormula20" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula200" hidden="1">_xll.Formula.SK('[7]Notes Data'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula201" hidden="1">_xll.Formula.SK([12]Formats!$J$5,1)</definedName>
-    <definedName name="SheetKraftFormula202" hidden="1">_xll.Formula.SK([12]Formats!$K$11,)</definedName>
-    <definedName name="SheetKraftFormula203" hidden="1">_xll.Formula.SK([2]Stack!$FD$6,1)</definedName>
-    <definedName name="SheetKraftFormula204" hidden="1">_xll.Formula.SK('[4]Asset Master'!$AT$3,1)</definedName>
-    <definedName name="SheetKraftFormula205" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BU$4,1)</definedName>
-    <definedName name="SheetKraftFormula206" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BX$5,1)</definedName>
-    <definedName name="SheetKraftFormula207" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$CA$4,1)</definedName>
-    <definedName name="SheetKraftFormula208" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BY$4,1)</definedName>
-    <definedName name="SheetKraftFormula209" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$L$4,1)</definedName>
-    <definedName name="SheetKraftFormula21" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula210" hidden="1">_xll.Formula.SK('[13]Rating Master'!$O$8,1)</definedName>
-    <definedName name="SheetKraftFormula212" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BG$9,1)</definedName>
-    <definedName name="SheetKraftFormula214" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$H$1,1)</definedName>
-    <definedName name="SheetKraftFormula216" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BF$4,1)</definedName>
-    <definedName name="SheetKraftFormula217" hidden="1">_xll.Formula.SK('[13]Rating Master'!$S$9,1)</definedName>
-    <definedName name="SheetKraftFormula218" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$AY$4,1)</definedName>
-    <definedName name="SheetKraftFormula219" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$AW$4,1)</definedName>
-    <definedName name="SheetKraftFormula22" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula220" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BA$5,1)</definedName>
-    <definedName name="SheetKraftFormula221" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BB$5,1)</definedName>
-    <definedName name="SheetKraftFormula222" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$AL$8,1)</definedName>
-    <definedName name="SheetKraftFormula223" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$T$8,1)</definedName>
-    <definedName name="SheetKraftFormula224" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BM$9,1)</definedName>
-    <definedName name="SheetKraftFormula225" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$M$4,1)</definedName>
-    <definedName name="SheetKraftFormula226" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$N$5,1)</definedName>
-    <definedName name="SheetKraftFormula227" hidden="1">_xll.Formula.SK('[15]Issuer Master'!$S$9,1)</definedName>
-    <definedName name="SheetKraftFormula228" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula229" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DE$9,1)</definedName>
-    <definedName name="SheetKraftFormula23" hidden="1">_xll.Formula.SK('[16]Security Master'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula230" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CI$9,1)</definedName>
-    <definedName name="SheetKraftFormula231" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CH$10,1)</definedName>
-    <definedName name="SheetKraftFormula232" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CY$10,1)</definedName>
-    <definedName name="SheetKraftFormula233" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$E$8,1)</definedName>
-    <definedName name="SheetKraftFormula234" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$L$8,1)</definedName>
-    <definedName name="SheetKraftFormula235" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$M$7,1)</definedName>
-    <definedName name="SheetKraftFormula236" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$N$6,1)</definedName>
-    <definedName name="SheetKraftFormula237" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$P$7,1)</definedName>
-    <definedName name="SheetKraftFormula238" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$K$7,1)</definedName>
-    <definedName name="SheetKraftFormula239" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$Q$7,1)</definedName>
-    <definedName name="SheetKraftFormula240" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$U$6,1)</definedName>
-    <definedName name="SheetKraftFormula241" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$T$10,1)</definedName>
-    <definedName name="SheetKraftFormula242" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$V$10,1)</definedName>
-    <definedName name="SheetKraftFormula243" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$Z$8,)</definedName>
-    <definedName name="SheetKraftFormula244" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AA$7,1)</definedName>
-    <definedName name="SheetKraftFormula245" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AB$6,)</definedName>
-    <definedName name="SheetKraftFormula246" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AD$7,1)</definedName>
-    <definedName name="SheetKraftFormula247" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$Y$7,1)</definedName>
-    <definedName name="SheetKraftFormula248" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AE$7,1)</definedName>
-    <definedName name="SheetKraftFormula249" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AI$6,1)</definedName>
-    <definedName name="SheetKraftFormula250" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AH$10,1)</definedName>
-    <definedName name="SheetKraftFormula251" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AJ$10,1)</definedName>
-    <definedName name="SheetKraftFormula252" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AL$2,)</definedName>
-    <definedName name="SheetKraftFormula253" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AO$6,1)</definedName>
-    <definedName name="SheetKraftFormula254" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AS$6,1)</definedName>
-    <definedName name="SheetKraftFormula255" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AT$6,1)</definedName>
-    <definedName name="SheetKraftFormula256" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AU$7,1)</definedName>
-    <definedName name="SheetKraftFormula258" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BG$6,1)</definedName>
-    <definedName name="SheetKraftFormula259" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AY$6,1)</definedName>
-    <definedName name="SheetKraftFormula26" hidden="1">_xll.Formula.SK('[15]Issuer Master'!$D$8,1)</definedName>
-    <definedName name="SheetKraftFormula260" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BM$6,1)</definedName>
-    <definedName name="SheetKraftFormula261" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BO$7,1)</definedName>
-    <definedName name="SheetKraftFormula262" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula263" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BH$6,1)</definedName>
-    <definedName name="SheetKraftFormula264" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BS$5,1)</definedName>
-    <definedName name="SheetKraftFormula265" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BI$6,1)</definedName>
-    <definedName name="SheetKraftFormula266" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BQ$6,1)</definedName>
-    <definedName name="SheetKraftFormula267" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BF$6,)</definedName>
-    <definedName name="SheetKraftFormula268" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BO$6,)</definedName>
-    <definedName name="SheetKraftFormula269" hidden="1">_xll.Formula.SK('[7]Notes Data'!$AK$9,1)</definedName>
-    <definedName name="SheetKraftFormula27" hidden="1">_xll.Formula.SK('[4]Asset Master'!$D$7,1)</definedName>
-    <definedName name="SheetKraftFormula270" hidden="1">_xll.Formula.SK('[7]Notes Data'!$AM$9,1)</definedName>
-    <definedName name="SheetKraftFormula271" hidden="1">_xll.Formula.SK('[7]Notes Data'!$AO$9,1)</definedName>
-    <definedName name="SheetKraftFormula272" hidden="1">_xll.Formula.SK('[7]Notes Data'!$AP$9,1)</definedName>
-    <definedName name="SheetKraftFormula273" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$AB$8,1)</definedName>
-    <definedName name="SheetKraftFormula274" hidden="1">_xll.Formula.SK('[1]Holding Positions'!$V$10,1)</definedName>
-    <definedName name="SheetKraftFormula275" hidden="1">_xll.Formula.SK('[18]Pre Working'!$D$6,1)</definedName>
-    <definedName name="SheetKraftFormula276" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DK$9,1)</definedName>
-    <definedName name="SheetKraftFormula277" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CF$9,1)</definedName>
-    <definedName name="SheetKraftFormula278" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CL$10,1)</definedName>
-    <definedName name="SheetKraftFormula279" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BS$6,1)</definedName>
-    <definedName name="SheetKraftFormula28" hidden="1">_xll.Formula.SK([8]Derivatives!$B$10,)</definedName>
-    <definedName name="SheetKraftFormula280" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BU$7,1)</definedName>
-    <definedName name="SheetKraftFormula281" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$BY$6,1)</definedName>
-    <definedName name="SheetKraftFormula282" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$CA$7,1)</definedName>
-    <definedName name="SheetKraftFormula283" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BN$9,1)</definedName>
-    <definedName name="SheetKraftFormula284" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BO$9,1)</definedName>
-    <definedName name="SheetKraftFormula285" hidden="1">_xll.Formula.SK([9]Inputs!$W$3,1)</definedName>
-    <definedName name="SheetKraftFormula286" hidden="1">_xll.Formula.SK([9]Inputs!$X$3,1)</definedName>
-    <definedName name="SheetKraftFormula287" hidden="1">_xll.Formula.SK([9]Inputs!$Z$4,1)</definedName>
-    <definedName name="SheetKraftFormula288" hidden="1">_xll.Formula.SK([9]Inputs!$AC$3,1)</definedName>
-    <definedName name="SheetKraftFormula289" hidden="1">_xll.Formula.SK([9]Inputs!$AD$4,1)</definedName>
-    <definedName name="SheetKraftFormula29" hidden="1">_xll.Formula.SK([8]Derivatives!$L$11,)</definedName>
-    <definedName name="SheetKraftFormula290" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DQ$9,1)</definedName>
-    <definedName name="SheetKraftFormula291" hidden="1">_xll.Formula.SK('[7]Notes Data'!#REF!,)</definedName>
-    <definedName name="SheetKraftFormula292" hidden="1">_xll.Formula.SK([9]Inputs!$AE$3,1)</definedName>
-    <definedName name="SheetKraftFormula293" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DR$9,1)</definedName>
-    <definedName name="SheetKraftFormula294" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DS$9,)</definedName>
-    <definedName name="SheetKraftFormula295" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DW$9,1)</definedName>
-    <definedName name="SheetKraftFormula296" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DV$9,)</definedName>
-    <definedName name="SheetKraftFormula298" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EB$9,)</definedName>
-    <definedName name="SheetKraftFormula299" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EA$9,)</definedName>
-    <definedName name="SheetKraftFormula3" hidden="1">_xll.Formula.SK('[10]Scheme Master'!$B$5,)</definedName>
-    <definedName name="SheetKraftFormula30" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$C$7,)</definedName>
-    <definedName name="SheetKraftFormula300" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EC$9,)</definedName>
-    <definedName name="SheetKraftFormula301" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EH$9,1)</definedName>
-    <definedName name="SheetKraftFormula302" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EG$9,)</definedName>
-    <definedName name="SheetKraftFormula303" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EE$9,1)</definedName>
-    <definedName name="SheetKraftFormula304" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EI$10,1)</definedName>
-    <definedName name="SheetKraftFormula305" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DB$1,)</definedName>
-    <definedName name="SheetKraftFormula306" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DG$19,1)</definedName>
-    <definedName name="SheetKraftFormula308" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EM$9,)</definedName>
-    <definedName name="SheetKraftFormula309" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EL$9,1)</definedName>
-    <definedName name="SheetKraftFormula31" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$I$7,)</definedName>
-    <definedName name="SheetKraftFormula310" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EO$10,1)</definedName>
-    <definedName name="SheetKraftFormula311" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EL$19,1)</definedName>
-    <definedName name="SheetKraftFormula312" hidden="1">_xll.Formula.SK('[7]Notes Data'!$ET$9,1)</definedName>
-    <definedName name="SheetKraftFormula313" hidden="1">_xll.Formula.SK('[7]Notes Data'!$ES$9,)</definedName>
-    <definedName name="SheetKraftFormula314" hidden="1">_xll.Formula.SK('[7]Notes Data'!$ER$9,1)</definedName>
-    <definedName name="SheetKraftFormula315" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EU$10,1)</definedName>
-    <definedName name="SheetKraftFormula316" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FH$9,1)</definedName>
-    <definedName name="SheetKraftFormula317" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FG$9,)</definedName>
-    <definedName name="SheetKraftFormula318" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FF$9,1)</definedName>
-    <definedName name="SheetKraftFormula319" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FI$10,1)</definedName>
-    <definedName name="SheetKraftFormula32" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$O$8,)</definedName>
-    <definedName name="SheetKraftFormula320" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FN$9,1)</definedName>
-    <definedName name="SheetKraftFormula321" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FL$1,)</definedName>
-    <definedName name="SheetKraftFormula322" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FU$9,1)</definedName>
-    <definedName name="SheetKraftFormula323" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FT$10,1)</definedName>
-    <definedName name="SheetKraftFormula324" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FW$10,1)</definedName>
-    <definedName name="SheetKraftFormula325" hidden="1">_xll.Formula.SK([2]Stack!$AX$1,1)</definedName>
-    <definedName name="SheetKraftFormula326" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$AC$8,1)</definedName>
-    <definedName name="SheetKraftFormula327" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$C$4,)</definedName>
-    <definedName name="SheetKraftFormula328" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$D$4,1)</definedName>
-    <definedName name="SheetKraftFormula329" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$E$4,)</definedName>
-    <definedName name="SheetKraftFormula33" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$S$8,1)</definedName>
-    <definedName name="SheetKraftFormula330" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$H$4,1)</definedName>
-    <definedName name="SheetKraftFormula331" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$J$4,)</definedName>
-    <definedName name="SheetKraftFormula332" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$N$4,)</definedName>
-    <definedName name="SheetKraftFormula333" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$L$4,)</definedName>
-    <definedName name="SheetKraftFormula334" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$O$4,)</definedName>
-    <definedName name="SheetKraftFormula335" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$P$4,)</definedName>
-    <definedName name="SheetKraftFormula336" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$Q$4,)</definedName>
-    <definedName name="SheetKraftFormula337" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$R$4,)</definedName>
-    <definedName name="SheetKraftFormula338" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$S$4,)</definedName>
-    <definedName name="SheetKraftFormula339" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$H$1,)</definedName>
-    <definedName name="SheetKraftFormula34" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$U$8,1)</definedName>
-    <definedName name="SheetKraftFormula340" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$AJ$4,)</definedName>
-    <definedName name="SheetKraftFormula341" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$AK$4,)</definedName>
-    <definedName name="SheetKraftFormula342" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$AM$4,)</definedName>
-    <definedName name="SheetKraftFormula343" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$AN$4,)</definedName>
-    <definedName name="SheetKraftFormula345" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$AP$4,)</definedName>
-    <definedName name="SheetKraftFormula346" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$AQ$4,)</definedName>
-    <definedName name="SheetKraftFormula347" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$I$4,)</definedName>
-    <definedName name="SheetKraftFormula348" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$AB$4,)</definedName>
-    <definedName name="SheetKraftFormula349" hidden="1">_xll.Formula.SK([2]Stack!$D$5,1)</definedName>
-    <definedName name="SheetKraftFormula35" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$V$8,1)</definedName>
-    <definedName name="SheetKraftFormula350" hidden="1">_xll.Formula.SK([2]Stack!$BE$6,1)</definedName>
-    <definedName name="SheetKraftFormula351" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$O$4,)</definedName>
-    <definedName name="SheetKraftFormula352" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$P$4,)</definedName>
-    <definedName name="SheetKraftFormula353" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$Q$4,)</definedName>
-    <definedName name="SheetKraftFormula354" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$R$4,)</definedName>
-    <definedName name="SheetKraftFormula355" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AB$4,)</definedName>
-    <definedName name="SheetKraftFormula357" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$A$2,1)</definedName>
-    <definedName name="SheetKraftFormula358" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$A$7,1)</definedName>
-    <definedName name="SheetKraftFormula36" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$W$9,)</definedName>
-    <definedName name="SheetKraftFormula360" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$A$4,)</definedName>
-    <definedName name="SheetKraftFormula361" hidden="1">_xll.Formula.SK('[19]Repo Rows'!$AL$4,)</definedName>
-    <definedName name="SheetKraftFormula362" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AO$4,)</definedName>
-    <definedName name="SheetKraftFormula363" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$A$2,)</definedName>
-    <definedName name="SheetKraftFormula364" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$A$5,)</definedName>
-    <definedName name="SheetKraftFormula365" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$A$7,)</definedName>
-    <definedName name="SheetKraftFormula366" hidden="1">_xll.Formula.SK('[20]Asset Pivots Grouping'!$G$12,1)</definedName>
-    <definedName name="SheetKraftFormula367" hidden="1">_xll.Formula.SK('[20]Asset Pivots Grouping'!$P$4,1)</definedName>
-    <definedName name="SheetKraftFormula368" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$R$1,1)</definedName>
-    <definedName name="SheetKraftFormula369" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$Q$4,1)</definedName>
-    <definedName name="SheetKraftFormula37" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$X$9,)</definedName>
-    <definedName name="SheetKraftFormula370" hidden="1">_xll.Formula.SK('[7]Notes Data'!$GM$10,1)</definedName>
-    <definedName name="SheetKraftFormula371" hidden="1">_xll.Formula.SK('[7]Notes Data'!$GT$10,1)</definedName>
-    <definedName name="SheetKraftFormula372" hidden="1">_xll.Formula.SK('[7]Notes Data'!$GW$10,1)</definedName>
-    <definedName name="SheetKraftFormula373" hidden="1">_xll.Formula.SK('[7]Notes Data'!$HH$10,1)</definedName>
-    <definedName name="SheetKraftFormula374" hidden="1">_xll.Formula.SK('[7]Notes Data'!$HM$10,1)</definedName>
-    <definedName name="SheetKraftFormula375" hidden="1">_xll.Formula.SK('[7]Notes Data'!$HR$10,1)</definedName>
-    <definedName name="SheetKraftFormula376" hidden="1">_xll.Formula.SK('[7]Notes Data'!$HP$10,1)</definedName>
-    <definedName name="SheetKraftFormula377" hidden="1">_xll.Formula.SK('[7]Notes Data'!$HQ$11,1)</definedName>
-    <definedName name="SheetKraftFormula378" hidden="1">_xll.Formula.SK('[7]Notes Data'!$HW$11,1)</definedName>
-    <definedName name="SheetKraftFormula379" hidden="1">_xll.Formula.SK('[13]Rating Master'!$E$8,1)</definedName>
-    <definedName name="SheetKraftFormula38" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$Y$9,)</definedName>
-    <definedName name="SheetKraftFormula380" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BT$9,1)</definedName>
-    <definedName name="SheetKraftFormula381" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BY$9,1)</definedName>
-    <definedName name="SheetKraftFormula382" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BX$9,)</definedName>
-    <definedName name="SheetKraftFormula383" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BZ$9,)</definedName>
-    <definedName name="SheetKraftFormula384" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CC$9,)</definedName>
-    <definedName name="SheetKraftFormula385" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CH$9,1)</definedName>
-    <definedName name="SheetKraftFormula386" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CE$10,1)</definedName>
-    <definedName name="SheetKraftFormula387" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CG$10,1)</definedName>
-    <definedName name="SheetKraftFormula388" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CL$9,1)</definedName>
-    <definedName name="SheetKraftFormula389" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CT$9,1)</definedName>
-    <definedName name="SheetKraftFormula39" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$Q$8,)</definedName>
-    <definedName name="SheetKraftFormula390" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CV$9,)</definedName>
-    <definedName name="SheetKraftFormula391" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CY$9,1)</definedName>
-    <definedName name="SheetKraftFormula392" hidden="1">_xll.Formula.SK('[21]No filter Class Master'!$H$11,1)</definedName>
-    <definedName name="SheetKraftFormula393" hidden="1">_xll.Formula.SK('[7]Notes Data'!$S$10,1)</definedName>
-    <definedName name="SheetKraftFormula394" hidden="1">_xll.Formula.SK('[22]Yes Bank Filter'!$H$9,1)</definedName>
-    <definedName name="SheetKraftFormula395" hidden="1">_xll.Formula.SK('[7]Notes Data'!$A$9,1)</definedName>
-    <definedName name="SheetKraftFormula396" hidden="1">_xll.Formula.SK('[7]Notes Data'!$T$9,1)</definedName>
-    <definedName name="SheetKraftFormula397" hidden="1">_xll.Formula.SK('[7]Notes Data'!$U$9,1)</definedName>
-    <definedName name="SheetKraftFormula398" hidden="1">_xll.Formula.SK('[7]Notes Data'!$AT$9,1)</definedName>
-    <definedName name="SheetKraftFormula399" hidden="1">_xll.Formula.SK('[7]Notes Data'!$AS$9,)</definedName>
-    <definedName name="SheetKraftFormula4" hidden="1">_xll.Formula.SK('[10]Scheme Master'!$B$6,1)</definedName>
-    <definedName name="SheetKraftFormula40" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$AF$14,1)</definedName>
-    <definedName name="SheetKraftFormula401" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BA$9,1)</definedName>
-    <definedName name="SheetKraftFormula404" hidden="1">_xll.Formula.SK('[7]Notes Data'!$V$10,1)</definedName>
-    <definedName name="SheetKraftFormula405" hidden="1">_xll.Formula.SK('[7]Notes Data'!$AZ$10,1)</definedName>
-    <definedName name="SheetKraftFormula406" hidden="1">_xll.Formula.SK('[7]Notes Data'!$AR$10,1)</definedName>
-    <definedName name="SheetKraftFormula407" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$F$9,1)</definedName>
-    <definedName name="SheetKraftFormula408" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$M$9,1)</definedName>
-    <definedName name="SheetKraftFormula409" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$E$10,1)</definedName>
-    <definedName name="SheetKraftFormula41" hidden="1">_xll.Formula.SK([8]Derivatives!$M$10,1)</definedName>
-    <definedName name="SheetKraftFormula410" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$R$9,1)</definedName>
-    <definedName name="SheetKraftFormula411" hidden="1">_xll.Formula.SK('[7]Notes Data'!$K$9,1)</definedName>
-    <definedName name="SheetKraftFormula412" hidden="1">_xll.Formula.SK('[24]Avg Yield'!$G$17,1)</definedName>
-    <definedName name="SheetKraftFormula413" hidden="1">_xll.Formula.SK('[24]Avg Yield'!$T$17,1)</definedName>
-    <definedName name="SheetKraftFormula414" hidden="1">_xll.Formula.SK([2]Stack!$FF$5,1)</definedName>
-    <definedName name="SheetKraftFormula415" hidden="1">_xll.Formula.SK([2]Stack!$FG$5,1)</definedName>
-    <definedName name="SheetKraftFormula416" hidden="1">_xll.Formula.SK([2]Stack!$FE$6,1)</definedName>
-    <definedName name="SheetKraftFormula417" hidden="1">_xll.Formula.SK([2]Stack!$FH$5,1)</definedName>
-    <definedName name="SheetKraftFormula418" hidden="1">_xll.Formula.SK([2]Stack!$FL$5,1)</definedName>
-    <definedName name="SheetKraftFormula419" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$J$14,)</definedName>
-    <definedName name="SheetKraftFormula42" hidden="1">_xll.Formula.SK([8]Derivatives!$N$11,)</definedName>
-    <definedName name="SheetKraftFormula420" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$I$15,)</definedName>
-    <definedName name="SheetKraftFormula421" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$G$14,)</definedName>
-    <definedName name="SheetKraftFormula422" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$F$14,)</definedName>
-    <definedName name="SheetKraftFormula423" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$H$15,)</definedName>
-    <definedName name="SheetKraftFormula424" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$C$15,)</definedName>
-    <definedName name="SheetKraftFormula425" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$D$15,)</definedName>
-    <definedName name="SheetKraftFormula426" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$E$15,)</definedName>
-    <definedName name="SheetKraftFormula427" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$B$15,)</definedName>
-    <definedName name="SheetKraftFormula428" hidden="1">_xll.Formula.SK([2]Stack!$C$5,1)</definedName>
-    <definedName name="SheetKraftFormula429" hidden="1">_xll.Formula.SK('[24]Avg Yield'!$Z$17,1)</definedName>
-    <definedName name="SheetKraftFormula43" hidden="1">_xll.Formula.SK('[18]Pre Working'!$E$4,1)</definedName>
-    <definedName name="SheetKraftFormula430" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EM$22,1)</definedName>
-    <definedName name="SheetKraftFormula431" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EN$9,)</definedName>
-    <definedName name="SheetKraftFormula432" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AE$9,1)</definedName>
-    <definedName name="SheetKraftFormula433" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AC$9,)</definedName>
-    <definedName name="SheetKraftFormula434" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AD$9,)</definedName>
-    <definedName name="SheetKraftFormula435" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AF$9,)</definedName>
-    <definedName name="SheetKraftFormula436" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AG$9,)</definedName>
-    <definedName name="SheetKraftFormula437" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AH$9,)</definedName>
-    <definedName name="SheetKraftFormula438" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AI$9,)</definedName>
-    <definedName name="SheetKraftFormula439" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AJ$9,)</definedName>
-    <definedName name="SheetKraftFormula44" hidden="1">_xll.Formula.SK('[1]Holding Positions'!$R$10,1)</definedName>
-    <definedName name="SheetKraftFormula440" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AM$9,1)</definedName>
-    <definedName name="SheetKraftFormula441" hidden="1">_xll.Formula.SK('[7]Notes Data'!$J$10,1)</definedName>
-    <definedName name="SheetKraftFormula442" hidden="1">_xll.Formula.SK('[7]Notes Data'!$H$10,1)</definedName>
-    <definedName name="SheetKraftFormula443" hidden="1">_xll.Formula.SK('[26]Liquid Schemes Working Day'!$I$11,)</definedName>
-    <definedName name="SheetKraftFormula444" hidden="1">_xll.Formula.SK('[26]Liquid Schemes Working Day'!$J$12,)</definedName>
-    <definedName name="SheetKraftFormula445" hidden="1">_xll.Formula.SK('[26]Liquid Schemes Working Day'!$K$12,)</definedName>
-    <definedName name="SheetKraftFormula446" hidden="1">_xll.Formula.SK('[26]Liquid Schemes Working Day'!$L$12,)</definedName>
-    <definedName name="SheetKraftFormula447" hidden="1">_xll.Formula.SK('[26]Liquid Schemes Working Day'!$P$11,1)</definedName>
-    <definedName name="SheetKraftFormula448" hidden="1">_xll.Formula.SK('[26]Liquid Schemes Working Day'!$M$12,1)</definedName>
-    <definedName name="SheetKraftFormula449" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$U$10,)</definedName>
-    <definedName name="SheetKraftFormula45" hidden="1">_xll.Formula.SK('[1]Holding Positions'!$S$10,1)</definedName>
-    <definedName name="SheetKraftFormula450" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AI$10,)</definedName>
-    <definedName name="SheetKraftFormula451" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula452" hidden="1">_xll.Formula.SK([12]Formats!$G$21,1)</definedName>
-    <definedName name="SheetKraftFormula453" hidden="1">_xll.Formula.SK('[27]Riskometer Levels'!$G$18,1)</definedName>
-    <definedName name="SheetKraftFormula454" hidden="1">_xll.Formula.SK([2]Stack!$FM$5,1)</definedName>
-    <definedName name="SheetKraftFormula455" hidden="1">_xll.Formula.SK('[7]Notes Data'!$GC$9,)</definedName>
-    <definedName name="SheetKraftFormula456" hidden="1">_xll.Formula.SK('[7]Notes Data'!$GD$9,)</definedName>
-    <definedName name="SheetKraftFormula457" hidden="1">_xll.Formula.SK('[7]Notes Data'!$GB$9,)</definedName>
-    <definedName name="SheetKraftFormula458" hidden="1">_xll.Formula.SK('[7]Notes Data'!$GH$9,)</definedName>
-    <definedName name="SheetKraftFormula459" hidden="1">_xll.Formula.SK('[7]Notes Data'!$GG$9,)</definedName>
-    <definedName name="SheetKraftFormula460" hidden="1">_xll.Formula.SK('[7]Notes Data'!$GI$9,)</definedName>
-    <definedName name="SheetKraftFormula461" hidden="1">_xll.Formula.SK('[28]Avg YTC'!$E$13,)</definedName>
-    <definedName name="SheetKraftFormula462" hidden="1">_xll.Formula.SK('[28]Avg YTC'!$D$14,1)</definedName>
-    <definedName name="SheetKraftFormula463" hidden="1">_xll.Formula.SK([2]Stack!$FN$5,1)</definedName>
-    <definedName name="SheetKraftFormula464" hidden="1">_xll.Formula.SK('[22]Yes Bank Filter'!$Q$9,1)</definedName>
-    <definedName name="SheetKraftFormula465" hidden="1">_xll.Formula.SK('[22]Yes Bank Filter'!$S$9,1)</definedName>
-    <definedName name="SheetKraftFormula466" hidden="1">_xll.Formula.SK('[22]Yes Bank Filter'!$T$9,1)</definedName>
-    <definedName name="SheetKraftFormula467" hidden="1">_xll.Formula.SK([2]Stack!$B$5,1)</definedName>
-    <definedName name="SheetKraftFormula468" hidden="1">_xll.Formula.SK('[17]Month NAV Last Date Calc'!$AV$7,1)</definedName>
-    <definedName name="SheetKraftFormula469" hidden="1">_xll.Formula.SK('[24]Avg Yield'!$AI$13,1)</definedName>
-    <definedName name="SheetKraftFormula470" hidden="1">_xll.Formula.SK([2]Stack!$FO$5,1)</definedName>
-    <definedName name="SheetKraftFormula471" hidden="1">_xll.Formula.SK('[7]Notes Data'!$IC$10,1)</definedName>
-    <definedName name="SheetKraftFormula472" hidden="1">_xll.Formula.SK('[7]Notes Data'!$IB$10,)</definedName>
-    <definedName name="SheetKraftFormula473" hidden="1">_xll.Formula.SK('[7]Notes Data'!$IA$10,1)</definedName>
-    <definedName name="SheetKraftFormula474" hidden="1">_xll.Formula.SK('[7]Notes Data'!$HZ$10,1)</definedName>
-    <definedName name="SheetKraftFormula475" hidden="1">_xll.Formula.SK('[7]Notes Data'!$HY$11,1)</definedName>
-    <definedName name="SheetKraftFormula476" hidden="1">_xll.Formula.SK('[7]Notes Data'!$IE$11,1)</definedName>
-    <definedName name="SheetKraftFormula477" hidden="1">_xll.Formula.SK('[27]Riskometer Levels'!$L$18,1)</definedName>
-    <definedName name="SheetKraftFormula478" hidden="1">_xll.Formula.SK([2]Stack!$FP$5,1)</definedName>
-    <definedName name="SheetKraftFormula479" hidden="1">_xll.Formula.SK('[7]Notes Data'!$IF$10,1)</definedName>
-    <definedName name="SheetKraftFormula48" hidden="1">_xll.Formula.SK('[1]Holding Positions'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula480" hidden="1">_xll.Formula.SK('[7]Notes Data'!$II$10,1)</definedName>
-    <definedName name="SheetKraftFormula481" hidden="1">_xll.Formula.SK('[7]Notes Data'!$HC$10,1)</definedName>
-    <definedName name="SheetKraftFormula482" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BP$9,1)</definedName>
-    <definedName name="SheetKraftFormula483" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BQ$10,1)</definedName>
-    <definedName name="SheetKraftFormula484" hidden="1">_xll.Formula.SK('[7]Notes Data'!$BR$10,1)</definedName>
-    <definedName name="SheetKraftFormula486" hidden="1">_xll.Formula.SK('[24]Avg Yield'!$AZ$14,1)</definedName>
-    <definedName name="SheetKraftFormula487" hidden="1">_xll.Formula.SK([2]Stack!$FQ$5,1)</definedName>
-    <definedName name="SheetKraftFormula488" hidden="1">_xll.Formula.SK([8]Derivatives!$U$10,)</definedName>
-    <definedName name="SheetKraftFormula489" hidden="1">_xll.Formula.SK([8]Derivatives!$S$10,1)</definedName>
-    <definedName name="SheetKraftFormula490" hidden="1">_xll.Formula.SK([8]Derivatives!$R$10,)</definedName>
-    <definedName name="SheetKraftFormula491" hidden="1">_xll.Formula.SK([9]Inputs!$N$14,1)</definedName>
-    <definedName name="SheetKraftFormula492" hidden="1">_xll.Formula.SK([9]Inputs!$N$6,)</definedName>
-    <definedName name="SheetKraftFormula493" hidden="1">_xll.Formula.SK([2]Stack!$FR$6,1)</definedName>
-    <definedName name="SheetKraftFormula494" hidden="1">_xll.Formula.SK([2]Stack!$GB$8,1)</definedName>
-    <definedName name="SheetKraftFormula495" hidden="1">_xll.Formula.SK([2]Stack!$FS$5,1)</definedName>
-    <definedName name="SheetKraftFormula496" hidden="1">_xll.Formula.SK('[7]Notes Data'!$IO$10,1)</definedName>
-    <definedName name="SheetKraftFormula497" hidden="1">_xll.Formula.SK('[7]Notes Data'!$IP$10,)</definedName>
-    <definedName name="SheetKraftFormula498" hidden="1">_xll.Formula.SK('[29]Foreign Securities'!$E$8,1)</definedName>
-    <definedName name="SheetKraftFormula499" hidden="1">_xll.Formula.SK('[29]Foreign Securities'!$J$8,1)</definedName>
-    <definedName name="SheetKraftFormula5" hidden="1">_xll.Formula.SK('[1]Holding Positions'!$L$10,1)</definedName>
-    <definedName name="SheetKraftFormula50" hidden="1">_xll.Formula.SK('[1]Holding Positions'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula500" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DY$9,1)</definedName>
-    <definedName name="SheetKraftFormula501" hidden="1">_xll.Formula.SK('[7]Notes Data'!$DX$10,1)</definedName>
-    <definedName name="SheetKraftFormula502" hidden="1">_xll.Formula.SK([2]Stack!$BD$5,1)</definedName>
-    <definedName name="SheetKraftFormula503" hidden="1">_xll.Formula.SK([2]Stack!$BD$6,1)</definedName>
-    <definedName name="SheetKraftFormula504" hidden="1">_xll.Formula.SK('[7]Notes Data'!$CX$9,1)</definedName>
-    <definedName name="SheetKraftFormula506" hidden="1">_xll.Formula.SK([2]Stack!$FT$5,1)</definedName>
-    <definedName name="SheetKraftFormula507" hidden="1">_xll.Formula.SK([2]Stack!$DG$5,1)</definedName>
-    <definedName name="SheetKraftFormula508" hidden="1">_xll.Formula.SK([2]Stack!$GG$8,1)</definedName>
-    <definedName name="SheetKraftFormula509" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$CE$4,1)</definedName>
-    <definedName name="SheetKraftFormula51" hidden="1">_xll.Formula.SK('[1]Holding Positions'!#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula510" hidden="1">_xll.Formula.SK('[30]Management Group'!$B$6,1)</definedName>
-    <definedName name="SheetKraftFormula511" hidden="1">_xll.Formula.SK([2]Stack!$FU$5,1)</definedName>
-    <definedName name="SheetKraftFormula512" hidden="1">_xll.Formula.SK([2]Stack!$GP$8,1)</definedName>
-    <definedName name="SheetKraftFormula513" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$CJ$4,1)</definedName>
-    <definedName name="SheetKraftFormula514" hidden="1">_xll.Formula.SK([2]Stack!$GX$8,1)</definedName>
-    <definedName name="SheetKraftFormula515" hidden="1">_xll.Formula.SK([2]Stack!$GX$1,1)</definedName>
-    <definedName name="SheetKraftFormula516" hidden="1">_xll.Formula.SK('[15]Issuer Master'!$W$10,)</definedName>
-    <definedName name="SheetKraftFormula517" hidden="1">_xll.Formula.SK('[25]Perpetual &amp; BT2'!$A$15,1)</definedName>
-    <definedName name="SheetKraftFormula518" hidden="1">_xll.Formula.SK([2]Stack!$DD$5,1)</definedName>
-    <definedName name="SheetKraftFormula519" hidden="1">_xll.Formula.SK('[7]Notes Data'!$IV$10,)</definedName>
-    <definedName name="SheetKraftFormula52" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula520" hidden="1">_xll.Formula.SK('[7]Notes Data'!$IY$11,)</definedName>
-    <definedName name="SheetKraftFormula521" hidden="1">_xll.Formula.SK('[7]Notes Data'!$JC$10,)</definedName>
-    <definedName name="SheetKraftFormula522" hidden="1">_xll.Formula.SK('[7]Notes Data'!$JF$11,)</definedName>
-    <definedName name="SheetKraftFormula523" hidden="1">_xll.Formula.SK('[31]Avg Yield Annualised'!$D$11,1)</definedName>
-    <definedName name="SheetKraftFormula524" hidden="1">_xll.Formula.SK([2]Stack!$FV$5,1)</definedName>
-    <definedName name="SheetKraftFormula525" hidden="1">_xll.Formula.SK('[16]Security Master'!$Z$9,1)</definedName>
-    <definedName name="SheetKraftFormula527" hidden="1">_xll.Formula.SK([8]Derivatives!$O$11,1)</definedName>
-    <definedName name="SheetKraftFormula528" hidden="1">_xll.Formula.SK([2]Stack!$FJ$6,1)</definedName>
-    <definedName name="SheetKraftFormula529" hidden="1">_xll.Formula.SK([2]Stack!$FK$6,1)</definedName>
-    <definedName name="SheetKraftFormula53" hidden="1">_xll.Formula.SK('[1]Holding Positions'!$V$12,1)</definedName>
-    <definedName name="SheetKraftFormula530" hidden="1">_xll.Formula.SK('[32]IRS Data'!$E$11,1)</definedName>
-    <definedName name="SheetKraftFormula531" hidden="1">_xll.Formula.SK('[32]IRS Data'!$P$11,1)</definedName>
-    <definedName name="SheetKraftFormula532" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$B$5,1)</definedName>
-    <definedName name="SheetKraftFormula533" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$J$5,1)</definedName>
-    <definedName name="SheetKraftFormula534" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$G$5,)</definedName>
-    <definedName name="SheetKraftFormula535" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$P$5,1)</definedName>
-    <definedName name="SheetKraftFormula536" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$W$4,1)</definedName>
-    <definedName name="SheetKraftFormula537" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$AC$5,1)</definedName>
-    <definedName name="SheetKraftFormula538" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$AH$5,1)</definedName>
-    <definedName name="SheetKraftFormula539" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$AG$6,1)</definedName>
-    <definedName name="SheetKraftFormula54" hidden="1">_xll.Formula.SK('[1]Holding Positions'!$T$11,1)</definedName>
-    <definedName name="SheetKraftFormula540" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$AF$5,)</definedName>
-    <definedName name="SheetKraftFormula541" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$AO$6,1)</definedName>
-    <definedName name="SheetKraftFormula542" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$AP$6,1)</definedName>
-    <definedName name="SheetKraftFormula543" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$AQ$6,1)</definedName>
-    <definedName name="SheetKraftFormula544" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$AR$6,)</definedName>
-    <definedName name="SheetKraftFormula545" hidden="1">_xll.Formula.SK('[33]Debt Derivative'!$AV$13,1)</definedName>
-    <definedName name="SheetKraftFormula546" hidden="1">_xll.Formula.SK('[32]IRS Data'!$M$11,1)</definedName>
-    <definedName name="SheetKraftFormula547" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EZ$9,1)</definedName>
-    <definedName name="SheetKraftFormula548" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EY$9,)</definedName>
-    <definedName name="SheetKraftFormula549" hidden="1">_xll.Formula.SK([8]Derivatives!$AW$10,1)</definedName>
-    <definedName name="SheetKraftFormula55" hidden="1">_xll.Formula.SK('[18]Pre Working'!$E$5,1)</definedName>
-    <definedName name="SheetKraftFormula550" hidden="1">_xll.Formula.SK('[7]Notes Data'!$EW$9,1)</definedName>
-    <definedName name="SheetKraftFormula551" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FA$10,1)</definedName>
-    <definedName name="SheetKraftFormula552" hidden="1">_xll.Formula.SK('[7]Notes Data'!$FB$9,1)</definedName>
-    <definedName name="SheetKraftFormula553" hidden="1">_xll.Formula.SK([8]Derivatives!$T$10,)</definedName>
-    <definedName name="SheetKraftFormula554" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AY$9,1)</definedName>
-    <definedName name="SheetKraftFormula555" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AU$9,1)</definedName>
-    <definedName name="SheetKraftFormula556" hidden="1">_xll.Formula.SK('[4]Asset Master'!$I$8,1)</definedName>
-    <definedName name="SheetKraftFormula557" hidden="1">_xll.Formula.SK('[32]IRS Data'!$Y$11,1)</definedName>
-    <definedName name="SheetKraftFormula558" hidden="1">_xll.Formula.SK('[32]IRS Data'!$X$11,1)</definedName>
-    <definedName name="SheetKraftFormula559" hidden="1">_xll.Formula.SK('[32]IRS Data'!$U$11,1)</definedName>
-    <definedName name="SheetKraftFormula560" hidden="1">_xll.Formula.SK('[20]Asset Pivots Grouping'!$O$13,1)</definedName>
-    <definedName name="SheetKraftFormula561" hidden="1">_xll.Formula.SK('[20]Asset Pivots Grouping'!$P$13,)</definedName>
-    <definedName name="SheetKraftFormula562" hidden="1">_xll.Formula.SK('[6]Pivots Data'!$BC$5,1)</definedName>
-    <definedName name="SheetKraftFormula563" hidden="1">_xll.Formula.SK([9]Inputs!$AG$3,1)</definedName>
-    <definedName name="SheetKraftFormula564" hidden="1">_xll.Formula.SK([9]Inputs!$AJ$3,1)</definedName>
-    <definedName name="SheetKraftFormula565" hidden="1">_xll.Formula.SK('[7]Notes Data'!$X$10,1)</definedName>
-    <definedName name="SheetKraftFormula566" hidden="1">_xll.Formula.SK('[23]Notes Data 2'!$AV$10,1)</definedName>
-    <definedName name="SheetKraftFormula567" hidden="1">_xll.Formula.SK('[26]Liquid Schemes Working Day'!$N$12,1)</definedName>
-    <definedName name="SheetKraftFormula57" hidden="1">_xll.Formula.SK('[18]Pre Working'!$K$5,1)</definedName>
-    <definedName name="SheetKraftFormula58" hidden="1">_xll.Formula.SK('[7]Notes Data'!$B$9,1)</definedName>
-    <definedName name="SheetKraftFormula59" hidden="1">_xll.Formula.SK('[7]Notes Data'!$Z$9,1)</definedName>
-    <definedName name="SheetKraftFormula6" hidden="1">_xll.Formula.SK('[16]Security Master'!$C$8,1)</definedName>
-    <definedName name="SheetKraftFormula61" hidden="1">_xll.Formula.SK('[18]Pre Working'!$AC$5,1)</definedName>
-    <definedName name="SheetKraftFormula62" hidden="1">_xll.Formula.SK('[18]Pre Working'!$AL$5,1)</definedName>
-    <definedName name="SheetKraftFormula63" hidden="1">_xll.Formula.SK('[16]Security Master'!$X$8,1)</definedName>
-    <definedName name="SheetKraftFormula64" hidden="1">_xll.Formula.SK('[4]Asset Master'!$T$7,1)</definedName>
-    <definedName name="SheetKraftFormula65" hidden="1">_xll.Formula.SK('[4]Asset Master'!$P$6,1)</definedName>
-    <definedName name="SheetKraftFormula66" hidden="1">_xll.Formula.SK('[18]Pre Working'!$AN$5,1)</definedName>
-    <definedName name="SheetKraftFormula67" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$Z$8,1)</definedName>
-    <definedName name="SheetKraftFormula68" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula69" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula7" hidden="1">_xll.Formula.SK('[16]Security Master'!$U$9,1)</definedName>
-    <definedName name="SheetKraftFormula70" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula71" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula72" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula73" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula74" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula75" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula76" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula77" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula78" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula79" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula8" hidden="1">_xll.Formula.SK('[16]Security Master'!$V$9,1)</definedName>
-    <definedName name="SheetKraftFormula80" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula81" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula82" hidden="1">_xll.Formula.SK(#REF!,)</definedName>
-    <definedName name="SheetKraftFormula83" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula84" hidden="1">_xll.Formula.SK(#REF!,1)</definedName>
-    <definedName name="SheetKraftFormula85" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$D$4,1)</definedName>
-    <definedName name="SheetKraftFormula86" hidden="1">_xll.Formula.SK('[14]NCA Calc, Repo'!$Z$9,1)</definedName>
-    <definedName name="SheetKraftFormula87" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$H$4,1)</definedName>
-    <definedName name="SheetKraftFormula88" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AJ$4,)</definedName>
-    <definedName name="SheetKraftFormula89" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AK$4,)</definedName>
-    <definedName name="SheetKraftFormula9" hidden="1">_xll.Formula.SK('[16]Security Master'!$W$9,1)</definedName>
-    <definedName name="SheetKraftFormula90" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AM$4,1)</definedName>
-    <definedName name="SheetKraftFormula91" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$C$4,)</definedName>
-    <definedName name="SheetKraftFormula92" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$J$4,)</definedName>
-    <definedName name="SheetKraftFormula93" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$E$4,1)</definedName>
-    <definedName name="SheetKraftFormula95" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$N$4,)</definedName>
-    <definedName name="SheetKraftFormula96" hidden="1">_xll.Formula.SK('[5]NCA Rows'!$AN$4,)</definedName>
-    <definedName name="SheetKraftFormula98" hidden="1">_xll.Formula.SK([2]Stack!$E$4,1)</definedName>
-    <definedName name="SheetKraftFormula99" hidden="1">_xll.Formula.SK([2]Stack!$AT$5,1)</definedName>
+    <definedName name="SheetKraftFormula1" hidden="1">Formula.SK('[1]Holding Positions'!$E$10,1)</definedName>
+    <definedName name="SheetKraftFormula10" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula100" hidden="1">Formula.SK([2]Stack!$AV$6,1)</definedName>
+    <definedName name="SheetKraftFormula101" hidden="1">Formula.SK([2]Stack!$AW$6,1)</definedName>
+    <definedName name="SheetKraftFormula102" hidden="1">Formula.SK([2]Stack!$AX$6,1)</definedName>
+    <definedName name="SheetKraftFormula104" hidden="1">Formula.SK([2]Stack!$BG$5,1)</definedName>
+    <definedName name="SheetKraftFormula105" hidden="1">Formula.SK([2]Stack!$CZ$6,1)</definedName>
+    <definedName name="SheetKraftFormula106" hidden="1">Formula.SK([2]Stack!$DI$5,1)</definedName>
+    <definedName name="SheetKraftFormula107" hidden="1">Formula.SK([2]Stack!$DH$5,1)</definedName>
+    <definedName name="SheetKraftFormula108" hidden="1">Formula.SK([3]Template_Formula!$A$3,1)</definedName>
+    <definedName name="SheetKraftFormula109" hidden="1">Formula.SK('[4]Asset Master'!$Y$7,1)</definedName>
+    <definedName name="SheetKraftFormula11" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula110" hidden="1">Formula.SK([2]Stack!$FC$5,1)</definedName>
+    <definedName name="SheetKraftFormula111" hidden="1">Formula.SK('[4]Asset Master'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula112" hidden="1">Formula.SK('[4]Asset Master'!$AI$10,1)</definedName>
+    <definedName name="SheetKraftFormula113" hidden="1">Formula.SK([2]Stack!$DB$5,1)</definedName>
+    <definedName name="SheetKraftFormula114" hidden="1">Formula.SK([2]Stack!$BF$5,1)</definedName>
+    <definedName name="SheetKraftFormula115" hidden="1">Formula.SK([2]Stack!$AZ$6,1)</definedName>
+    <definedName name="SheetKraftFormula116" hidden="1">Formula.SK([2]Stack!$AY$5,1)</definedName>
+    <definedName name="SheetKraftFormula117" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula118" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula119" hidden="1">Formula.SK('[5]NCA Rows'!$R$5,1)</definedName>
+    <definedName name="SheetKraftFormula12" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula120" hidden="1">Formula.SK('[5]NCA Rows'!$AB$5,1)</definedName>
+    <definedName name="SheetKraftFormula121" hidden="1">Formula.SK([2]Stack!$BA$6,1)</definedName>
+    <definedName name="SheetKraftFormula123" hidden="1">Formula.SK('[5]NCA Rows'!$I$4,)</definedName>
+    <definedName name="SheetKraftFormula124" hidden="1">Formula.SK('[5]NCA Rows'!$L$4,)</definedName>
+    <definedName name="SheetKraftFormula125" hidden="1">Formula.SK('[5]NCA Rows'!$S$4,)</definedName>
+    <definedName name="SheetKraftFormula126" hidden="1">Formula.SK('[5]NCA Rows'!$AP$4,)</definedName>
+    <definedName name="SheetKraftFormula127" hidden="1">Formula.SK('[5]NCA Rows'!$AQ$4,)</definedName>
+    <definedName name="SheetKraftFormula128" hidden="1">Formula.SK('[5]NCA Rows'!$AX$4,1)</definedName>
+    <definedName name="SheetKraftFormula129" hidden="1">Formula.SK('[5]NCA Rows'!$AZ$5,1)</definedName>
+    <definedName name="SheetKraftFormula13" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula130" hidden="1">Formula.SK([2]Stack!$BB$5,1)</definedName>
+    <definedName name="SheetKraftFormula131" hidden="1">Formula.SK('[6]Pivots Data'!$B$4,1)</definedName>
+    <definedName name="SheetKraftFormula132" hidden="1">Formula.SK('[6]Pivots Data'!$H$4,1)</definedName>
+    <definedName name="SheetKraftFormula133" hidden="1">Formula.SK('[6]Pivots Data'!$J$5,1)</definedName>
+    <definedName name="SheetKraftFormula134" hidden="1">Formula.SK('[6]Pivots Data'!$BJ$4,1)</definedName>
+    <definedName name="SheetKraftFormula135" hidden="1">Formula.SK('[6]Pivots Data'!$AC$4,1)</definedName>
+    <definedName name="SheetKraftFormula136" hidden="1">Formula.SK('[6]Pivots Data'!$K$5,1)</definedName>
+    <definedName name="SheetKraftFormula137" hidden="1">Formula.SK([2]Stack!$DC$5,1)</definedName>
+    <definedName name="SheetKraftFormula138" hidden="1">Formula.SK('[6]Pivots Data'!$AP$4,1)</definedName>
+    <definedName name="SheetKraftFormula139" hidden="1">Formula.SK('[6]Pivots Data'!$BA$4,1)</definedName>
+    <definedName name="SheetKraftFormula14" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula140" hidden="1">Formula.SK('[6]Pivots Data'!$AI$4,1)</definedName>
+    <definedName name="SheetKraftFormula141" hidden="1">Formula.SK([3]Template_Formula!$A$10,1)</definedName>
+    <definedName name="SheetKraftFormula142" hidden="1">Formula.SK('[7]Notes Data'!$AH$9,1)</definedName>
+    <definedName name="SheetKraftFormula144" hidden="1">Formula.SK('[7]Notes Data'!$BF$9,1)</definedName>
+    <definedName name="SheetKraftFormula145" hidden="1">Formula.SK('[7]Notes Data'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula146" hidden="1">Formula.SK('[7]Notes Data'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula147" hidden="1">Formula.SK([3]Template_Formula!$A$16,1)</definedName>
+    <definedName name="SheetKraftFormula148" hidden="1">Formula.SK('[7]Notes Data'!$BI$9,1)</definedName>
+    <definedName name="SheetKraftFormula149" hidden="1">Formula.SK([3]Template_Formula!$A$15,1)</definedName>
+    <definedName name="SheetKraftFormula15" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula150" hidden="1">Formula.SK([3]Template_Formula!$O$9,1)</definedName>
+    <definedName name="SheetKraftFormula152" hidden="1">Formula.SK([8]Derivatives!$Y$10,1)</definedName>
+    <definedName name="SheetKraftFormula153" hidden="1">Formula.SK([8]Derivatives!$AA$11,1)</definedName>
+    <definedName name="SheetKraftFormula154" hidden="1">Formula.SK([8]Derivatives!$AB$11,1)</definedName>
+    <definedName name="SheetKraftFormula155" hidden="1">Formula.SK([3]Template_Formula!$O$14,1)</definedName>
+    <definedName name="SheetKraftFormula156" hidden="1">Formula.SK([8]Derivatives!$AF$10,1)</definedName>
+    <definedName name="SheetKraftFormula157" hidden="1">Formula.SK([8]Derivatives!$AH$10,1)</definedName>
+    <definedName name="SheetKraftFormula158" hidden="1">Formula.SK([8]Derivatives!$AI$11,1)</definedName>
+    <definedName name="SheetKraftFormula159" hidden="1">Formula.SK([8]Derivatives!$AI$10,)</definedName>
+    <definedName name="SheetKraftFormula16" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula160" hidden="1">Formula.SK([8]Derivatives!$AJ$10,)</definedName>
+    <definedName name="SheetKraftFormula161" hidden="1">Formula.SK([8]Derivatives!$AK$10,)</definedName>
+    <definedName name="SheetKraftFormula162" hidden="1">Formula.SK([8]Derivatives!$AO$10,1)</definedName>
+    <definedName name="SheetKraftFormula163" hidden="1">Formula.SK('[6]Pivots Data'!$V$3,1)</definedName>
+    <definedName name="SheetKraftFormula164" hidden="1">Formula.SK('[7]Notes Data'!$CK$9,1)</definedName>
+    <definedName name="SheetKraftFormula165" hidden="1">Formula.SK('[7]Notes Data'!$CM$9,1)</definedName>
+    <definedName name="SheetKraftFormula167" hidden="1">Formula.SK('[7]Notes Data'!$CO$9,)</definedName>
+    <definedName name="SheetKraftFormula168" hidden="1">Formula.SK('[7]Notes Data'!$CN$9,)</definedName>
+    <definedName name="SheetKraftFormula169" hidden="1">Formula.SK('[7]Notes Data'!$CQ$9,1)</definedName>
+    <definedName name="SheetKraftFormula17" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula170" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula171" hidden="1">Formula.SK('[7]Notes Data'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula172" hidden="1">Formula.SK('[7]Notes Data'!$CR$9,1)</definedName>
+    <definedName name="SheetKraftFormula174" hidden="1">Formula.SK('[7]Notes Data'!$CU$10,1)</definedName>
+    <definedName name="SheetKraftFormula175" hidden="1">Formula.SK('[7]Notes Data'!$CV$10,1)</definedName>
+    <definedName name="SheetKraftFormula176" hidden="1">Formula.SK('[7]Notes Data'!$CW$9,)</definedName>
+    <definedName name="SheetKraftFormula177" hidden="1">Formula.SK('[7]Notes Data'!$CX$10,1)</definedName>
+    <definedName name="SheetKraftFormula178" hidden="1">Formula.SK('[7]Notes Data'!$CK$10,1)</definedName>
+    <definedName name="SheetKraftFormula179" hidden="1">Formula.SK('[7]Notes Data'!$CJ$10,1)</definedName>
+    <definedName name="SheetKraftFormula18" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula180" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula181" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula182" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula183" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula184" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula185" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula186" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula187" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula188" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula189" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula19" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula191" hidden="1">Formula.SK([9]Inputs!$Q$7,1)</definedName>
+    <definedName name="SheetKraftFormula192" hidden="1">Formula.SK('[10]Scheme Master'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula193" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula194" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula195" hidden="1">Formula.SK('[10]Scheme Master'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula196" hidden="1">Formula.SK('[10]Scheme Master'!$J$7,1)</definedName>
+    <definedName name="SheetKraftFormula197" hidden="1">Formula.SK('[11]Scheme Category'!$D$9,1)</definedName>
+    <definedName name="SheetKraftFormula198" hidden="1">Formula.SK('[7]Notes Data'!$BE$9,1)</definedName>
+    <definedName name="SheetKraftFormula199" hidden="1">Formula.SK('[7]Notes Data'!$BD$9,1)</definedName>
+    <definedName name="SheetKraftFormula20" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula200" hidden="1">Formula.SK('[7]Notes Data'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula201" hidden="1">Formula.SK([12]Formats!$J$5,1)</definedName>
+    <definedName name="SheetKraftFormula202" hidden="1">Formula.SK([12]Formats!$K$11,)</definedName>
+    <definedName name="SheetKraftFormula203" hidden="1">Formula.SK([2]Stack!$FD$6,1)</definedName>
+    <definedName name="SheetKraftFormula204" hidden="1">Formula.SK('[4]Asset Master'!$AT$3,1)</definedName>
+    <definedName name="SheetKraftFormula205" hidden="1">Formula.SK('[6]Pivots Data'!$BU$4,1)</definedName>
+    <definedName name="SheetKraftFormula206" hidden="1">Formula.SK('[6]Pivots Data'!$BX$5,1)</definedName>
+    <definedName name="SheetKraftFormula207" hidden="1">Formula.SK('[6]Pivots Data'!$CA$4,1)</definedName>
+    <definedName name="SheetKraftFormula208" hidden="1">Formula.SK('[6]Pivots Data'!$BY$4,1)</definedName>
+    <definedName name="SheetKraftFormula209" hidden="1">Formula.SK('[6]Pivots Data'!$L$4,1)</definedName>
+    <definedName name="SheetKraftFormula21" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula210" hidden="1">Formula.SK('[13]Rating Master'!$O$8,1)</definedName>
+    <definedName name="SheetKraftFormula212" hidden="1">Formula.SK('[6]Pivots Data'!$BG$9,1)</definedName>
+    <definedName name="SheetKraftFormula214" hidden="1">Formula.SK('[5]NCA Rows'!$H$1,1)</definedName>
+    <definedName name="SheetKraftFormula216" hidden="1">Formula.SK('[6]Pivots Data'!$BF$4,1)</definedName>
+    <definedName name="SheetKraftFormula217" hidden="1">Formula.SK('[13]Rating Master'!$S$9,1)</definedName>
+    <definedName name="SheetKraftFormula218" hidden="1">Formula.SK('[6]Pivots Data'!$AY$4,1)</definedName>
+    <definedName name="SheetKraftFormula219" hidden="1">Formula.SK('[6]Pivots Data'!$AW$4,1)</definedName>
+    <definedName name="SheetKraftFormula22" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula220" hidden="1">Formula.SK('[6]Pivots Data'!$BA$5,1)</definedName>
+    <definedName name="SheetKraftFormula221" hidden="1">Formula.SK('[6]Pivots Data'!$BB$5,1)</definedName>
+    <definedName name="SheetKraftFormula222" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$AL$8,1)</definedName>
+    <definedName name="SheetKraftFormula223" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$T$8,1)</definedName>
+    <definedName name="SheetKraftFormula224" hidden="1">Formula.SK('[7]Notes Data'!$BM$9,1)</definedName>
+    <definedName name="SheetKraftFormula225" hidden="1">Formula.SK('[6]Pivots Data'!$M$4,1)</definedName>
+    <definedName name="SheetKraftFormula226" hidden="1">Formula.SK('[6]Pivots Data'!$N$5,1)</definedName>
+    <definedName name="SheetKraftFormula227" hidden="1">Formula.SK('[15]Issuer Master'!$S$9,1)</definedName>
+    <definedName name="SheetKraftFormula228" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula229" hidden="1">Formula.SK('[7]Notes Data'!$DE$9,1)</definedName>
+    <definedName name="SheetKraftFormula23" hidden="1">Formula.SK('[16]Security Master'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula230" hidden="1">Formula.SK('[7]Notes Data'!$CI$9,1)</definedName>
+    <definedName name="SheetKraftFormula231" hidden="1">Formula.SK('[7]Notes Data'!$CH$10,1)</definedName>
+    <definedName name="SheetKraftFormula232" hidden="1">Formula.SK('[7]Notes Data'!$CY$10,1)</definedName>
+    <definedName name="SheetKraftFormula233" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$E$8,1)</definedName>
+    <definedName name="SheetKraftFormula234" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$L$8,1)</definedName>
+    <definedName name="SheetKraftFormula235" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$M$7,1)</definedName>
+    <definedName name="SheetKraftFormula236" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$N$6,1)</definedName>
+    <definedName name="SheetKraftFormula237" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$P$7,1)</definedName>
+    <definedName name="SheetKraftFormula238" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$K$7,1)</definedName>
+    <definedName name="SheetKraftFormula239" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$Q$7,1)</definedName>
+    <definedName name="SheetKraftFormula240" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$U$6,1)</definedName>
+    <definedName name="SheetKraftFormula241" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$T$10,1)</definedName>
+    <definedName name="SheetKraftFormula242" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$V$10,1)</definedName>
+    <definedName name="SheetKraftFormula243" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$Z$8,)</definedName>
+    <definedName name="SheetKraftFormula244" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AA$7,1)</definedName>
+    <definedName name="SheetKraftFormula245" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AB$6,)</definedName>
+    <definedName name="SheetKraftFormula246" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AD$7,1)</definedName>
+    <definedName name="SheetKraftFormula247" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$Y$7,1)</definedName>
+    <definedName name="SheetKraftFormula248" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AE$7,1)</definedName>
+    <definedName name="SheetKraftFormula249" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AI$6,1)</definedName>
+    <definedName name="SheetKraftFormula250" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AH$10,1)</definedName>
+    <definedName name="SheetKraftFormula251" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AJ$10,1)</definedName>
+    <definedName name="SheetKraftFormula252" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AL$2,)</definedName>
+    <definedName name="SheetKraftFormula253" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AO$6,1)</definedName>
+    <definedName name="SheetKraftFormula254" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AS$6,1)</definedName>
+    <definedName name="SheetKraftFormula255" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AT$6,1)</definedName>
+    <definedName name="SheetKraftFormula256" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AU$7,1)</definedName>
+    <definedName name="SheetKraftFormula258" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BG$6,1)</definedName>
+    <definedName name="SheetKraftFormula259" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AY$6,1)</definedName>
+    <definedName name="SheetKraftFormula26" hidden="1">Formula.SK('[15]Issuer Master'!$D$8,1)</definedName>
+    <definedName name="SheetKraftFormula260" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BM$6,1)</definedName>
+    <definedName name="SheetKraftFormula261" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BO$7,1)</definedName>
+    <definedName name="SheetKraftFormula262" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula263" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BH$6,1)</definedName>
+    <definedName name="SheetKraftFormula264" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BS$5,1)</definedName>
+    <definedName name="SheetKraftFormula265" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BI$6,1)</definedName>
+    <definedName name="SheetKraftFormula266" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BQ$6,1)</definedName>
+    <definedName name="SheetKraftFormula267" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BF$6,)</definedName>
+    <definedName name="SheetKraftFormula268" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BO$6,)</definedName>
+    <definedName name="SheetKraftFormula269" hidden="1">Formula.SK('[7]Notes Data'!$AK$9,1)</definedName>
+    <definedName name="SheetKraftFormula27" hidden="1">Formula.SK('[4]Asset Master'!$D$7,1)</definedName>
+    <definedName name="SheetKraftFormula270" hidden="1">Formula.SK('[7]Notes Data'!$AM$9,1)</definedName>
+    <definedName name="SheetKraftFormula271" hidden="1">Formula.SK('[7]Notes Data'!$AO$9,1)</definedName>
+    <definedName name="SheetKraftFormula272" hidden="1">Formula.SK('[7]Notes Data'!$AP$9,1)</definedName>
+    <definedName name="SheetKraftFormula273" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$AB$8,1)</definedName>
+    <definedName name="SheetKraftFormula274" hidden="1">Formula.SK('[1]Holding Positions'!$V$10,1)</definedName>
+    <definedName name="SheetKraftFormula275" hidden="1">Formula.SK('[18]Pre Working'!$D$6,1)</definedName>
+    <definedName name="SheetKraftFormula276" hidden="1">Formula.SK('[7]Notes Data'!$DK$9,1)</definedName>
+    <definedName name="SheetKraftFormula277" hidden="1">Formula.SK('[7]Notes Data'!$CF$9,1)</definedName>
+    <definedName name="SheetKraftFormula278" hidden="1">Formula.SK('[7]Notes Data'!$CL$10,1)</definedName>
+    <definedName name="SheetKraftFormula279" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BS$6,1)</definedName>
+    <definedName name="SheetKraftFormula28" hidden="1">Formula.SK([8]Derivatives!$B$10,)</definedName>
+    <definedName name="SheetKraftFormula280" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BU$7,1)</definedName>
+    <definedName name="SheetKraftFormula281" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$BY$6,1)</definedName>
+    <definedName name="SheetKraftFormula282" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$CA$7,1)</definedName>
+    <definedName name="SheetKraftFormula283" hidden="1">Formula.SK('[7]Notes Data'!$BN$9,1)</definedName>
+    <definedName name="SheetKraftFormula284" hidden="1">Formula.SK('[7]Notes Data'!$BO$9,1)</definedName>
+    <definedName name="SheetKraftFormula285" hidden="1">Formula.SK([9]Inputs!$W$3,1)</definedName>
+    <definedName name="SheetKraftFormula286" hidden="1">Formula.SK([9]Inputs!$X$3,1)</definedName>
+    <definedName name="SheetKraftFormula287" hidden="1">Formula.SK([9]Inputs!$Z$4,1)</definedName>
+    <definedName name="SheetKraftFormula288" hidden="1">Formula.SK([9]Inputs!$AC$3,1)</definedName>
+    <definedName name="SheetKraftFormula289" hidden="1">Formula.SK([9]Inputs!$AD$4,1)</definedName>
+    <definedName name="SheetKraftFormula29" hidden="1">Formula.SK([8]Derivatives!$L$11,)</definedName>
+    <definedName name="SheetKraftFormula290" hidden="1">Formula.SK('[7]Notes Data'!$DQ$9,1)</definedName>
+    <definedName name="SheetKraftFormula291" hidden="1">Formula.SK('[7]Notes Data'!#REF!,)</definedName>
+    <definedName name="SheetKraftFormula292" hidden="1">Formula.SK([9]Inputs!$AE$3,1)</definedName>
+    <definedName name="SheetKraftFormula293" hidden="1">Formula.SK('[7]Notes Data'!$DR$9,1)</definedName>
+    <definedName name="SheetKraftFormula294" hidden="1">Formula.SK('[7]Notes Data'!$DS$9,)</definedName>
+    <definedName name="SheetKraftFormula295" hidden="1">Formula.SK('[7]Notes Data'!$DW$9,1)</definedName>
+    <definedName name="SheetKraftFormula296" hidden="1">Formula.SK('[7]Notes Data'!$DV$9,)</definedName>
+    <definedName name="SheetKraftFormula298" hidden="1">Formula.SK('[7]Notes Data'!$EB$9,)</definedName>
+    <definedName name="SheetKraftFormula299" hidden="1">Formula.SK('[7]Notes Data'!$EA$9,)</definedName>
+    <definedName name="SheetKraftFormula3" hidden="1">Formula.SK('[10]Scheme Master'!$B$5,)</definedName>
+    <definedName name="SheetKraftFormula30" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$C$7,)</definedName>
+    <definedName name="SheetKraftFormula300" hidden="1">Formula.SK('[7]Notes Data'!$EC$9,)</definedName>
+    <definedName name="SheetKraftFormula301" hidden="1">Formula.SK('[7]Notes Data'!$EH$9,1)</definedName>
+    <definedName name="SheetKraftFormula302" hidden="1">Formula.SK('[7]Notes Data'!$EG$9,)</definedName>
+    <definedName name="SheetKraftFormula303" hidden="1">Formula.SK('[7]Notes Data'!$EE$9,1)</definedName>
+    <definedName name="SheetKraftFormula304" hidden="1">Formula.SK('[7]Notes Data'!$EI$10,1)</definedName>
+    <definedName name="SheetKraftFormula305" hidden="1">Formula.SK('[7]Notes Data'!$DB$1,)</definedName>
+    <definedName name="SheetKraftFormula306" hidden="1">Formula.SK('[7]Notes Data'!$DG$19,1)</definedName>
+    <definedName name="SheetKraftFormula308" hidden="1">Formula.SK('[7]Notes Data'!$EM$9,)</definedName>
+    <definedName name="SheetKraftFormula309" hidden="1">Formula.SK('[7]Notes Data'!$EL$9,1)</definedName>
+    <definedName name="SheetKraftFormula31" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$I$7,)</definedName>
+    <definedName name="SheetKraftFormula310" hidden="1">Formula.SK('[7]Notes Data'!$EO$10,1)</definedName>
+    <definedName name="SheetKraftFormula311" hidden="1">Formula.SK('[7]Notes Data'!$EL$19,1)</definedName>
+    <definedName name="SheetKraftFormula312" hidden="1">Formula.SK('[7]Notes Data'!$ET$9,1)</definedName>
+    <definedName name="SheetKraftFormula313" hidden="1">Formula.SK('[7]Notes Data'!$ES$9,)</definedName>
+    <definedName name="SheetKraftFormula314" hidden="1">Formula.SK('[7]Notes Data'!$ER$9,1)</definedName>
+    <definedName name="SheetKraftFormula315" hidden="1">Formula.SK('[7]Notes Data'!$EU$10,1)</definedName>
+    <definedName name="SheetKraftFormula316" hidden="1">Formula.SK('[7]Notes Data'!$FH$9,1)</definedName>
+    <definedName name="SheetKraftFormula317" hidden="1">Formula.SK('[7]Notes Data'!$FG$9,)</definedName>
+    <definedName name="SheetKraftFormula318" hidden="1">Formula.SK('[7]Notes Data'!$FF$9,1)</definedName>
+    <definedName name="SheetKraftFormula319" hidden="1">Formula.SK('[7]Notes Data'!$FI$10,1)</definedName>
+    <definedName name="SheetKraftFormula32" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$O$8,)</definedName>
+    <definedName name="SheetKraftFormula320" hidden="1">Formula.SK('[7]Notes Data'!$FN$9,1)</definedName>
+    <definedName name="SheetKraftFormula321" hidden="1">Formula.SK('[7]Notes Data'!$FL$1,)</definedName>
+    <definedName name="SheetKraftFormula322" hidden="1">Formula.SK('[7]Notes Data'!$FU$9,1)</definedName>
+    <definedName name="SheetKraftFormula323" hidden="1">Formula.SK('[7]Notes Data'!$FT$10,1)</definedName>
+    <definedName name="SheetKraftFormula324" hidden="1">Formula.SK('[7]Notes Data'!$FW$10,1)</definedName>
+    <definedName name="SheetKraftFormula325" hidden="1">Formula.SK([2]Stack!$AX$1,1)</definedName>
+    <definedName name="SheetKraftFormula326" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$AC$8,1)</definedName>
+    <definedName name="SheetKraftFormula327" hidden="1">Formula.SK('[19]Repo Rows'!$C$4,)</definedName>
+    <definedName name="SheetKraftFormula328" hidden="1">Formula.SK('[19]Repo Rows'!$D$4,1)</definedName>
+    <definedName name="SheetKraftFormula329" hidden="1">Formula.SK('[19]Repo Rows'!$E$4,)</definedName>
+    <definedName name="SheetKraftFormula33" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$S$8,1)</definedName>
+    <definedName name="SheetKraftFormula330" hidden="1">Formula.SK('[19]Repo Rows'!$H$4,1)</definedName>
+    <definedName name="SheetKraftFormula331" hidden="1">Formula.SK('[19]Repo Rows'!$J$4,)</definedName>
+    <definedName name="SheetKraftFormula332" hidden="1">Formula.SK('[19]Repo Rows'!$N$4,)</definedName>
+    <definedName name="SheetKraftFormula333" hidden="1">Formula.SK('[19]Repo Rows'!$L$4,)</definedName>
+    <definedName name="SheetKraftFormula334" hidden="1">Formula.SK('[19]Repo Rows'!$O$4,)</definedName>
+    <definedName name="SheetKraftFormula335" hidden="1">Formula.SK('[19]Repo Rows'!$P$4,)</definedName>
+    <definedName name="SheetKraftFormula336" hidden="1">Formula.SK('[19]Repo Rows'!$Q$4,)</definedName>
+    <definedName name="SheetKraftFormula337" hidden="1">Formula.SK('[19]Repo Rows'!$R$4,)</definedName>
+    <definedName name="SheetKraftFormula338" hidden="1">Formula.SK('[19]Repo Rows'!$S$4,)</definedName>
+    <definedName name="SheetKraftFormula339" hidden="1">Formula.SK('[19]Repo Rows'!$H$1,)</definedName>
+    <definedName name="SheetKraftFormula34" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$U$8,1)</definedName>
+    <definedName name="SheetKraftFormula340" hidden="1">Formula.SK('[19]Repo Rows'!$AJ$4,)</definedName>
+    <definedName name="SheetKraftFormula341" hidden="1">Formula.SK('[19]Repo Rows'!$AK$4,)</definedName>
+    <definedName name="SheetKraftFormula342" hidden="1">Formula.SK('[19]Repo Rows'!$AM$4,)</definedName>
+    <definedName name="SheetKraftFormula343" hidden="1">Formula.SK('[19]Repo Rows'!$AN$4,)</definedName>
+    <definedName name="SheetKraftFormula345" hidden="1">Formula.SK('[19]Repo Rows'!$AP$4,)</definedName>
+    <definedName name="SheetKraftFormula346" hidden="1">Formula.SK('[19]Repo Rows'!$AQ$4,)</definedName>
+    <definedName name="SheetKraftFormula347" hidden="1">Formula.SK('[19]Repo Rows'!$I$4,)</definedName>
+    <definedName name="SheetKraftFormula348" hidden="1">Formula.SK('[19]Repo Rows'!$AB$4,)</definedName>
+    <definedName name="SheetKraftFormula349" hidden="1">Formula.SK([2]Stack!$D$5,1)</definedName>
+    <definedName name="SheetKraftFormula35" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$V$8,1)</definedName>
+    <definedName name="SheetKraftFormula350" hidden="1">Formula.SK([2]Stack!$BE$6,1)</definedName>
+    <definedName name="SheetKraftFormula351" hidden="1">Formula.SK('[5]NCA Rows'!$O$4,)</definedName>
+    <definedName name="SheetKraftFormula352" hidden="1">Formula.SK('[5]NCA Rows'!$P$4,)</definedName>
+    <definedName name="SheetKraftFormula353" hidden="1">Formula.SK('[5]NCA Rows'!$Q$4,)</definedName>
+    <definedName name="SheetKraftFormula354" hidden="1">Formula.SK('[5]NCA Rows'!$R$4,)</definedName>
+    <definedName name="SheetKraftFormula355" hidden="1">Formula.SK('[5]NCA Rows'!$AB$4,)</definedName>
+    <definedName name="SheetKraftFormula357" hidden="1">Formula.SK('[19]Repo Rows'!$A$2,1)</definedName>
+    <definedName name="SheetKraftFormula358" hidden="1">Formula.SK('[19]Repo Rows'!$A$7,1)</definedName>
+    <definedName name="SheetKraftFormula36" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$W$9,)</definedName>
+    <definedName name="SheetKraftFormula360" hidden="1">Formula.SK('[19]Repo Rows'!$A$4,)</definedName>
+    <definedName name="SheetKraftFormula361" hidden="1">Formula.SK('[19]Repo Rows'!$AL$4,)</definedName>
+    <definedName name="SheetKraftFormula362" hidden="1">Formula.SK('[5]NCA Rows'!$AO$4,)</definedName>
+    <definedName name="SheetKraftFormula363" hidden="1">Formula.SK('[5]NCA Rows'!$A$2,)</definedName>
+    <definedName name="SheetKraftFormula364" hidden="1">Formula.SK('[5]NCA Rows'!$A$5,)</definedName>
+    <definedName name="SheetKraftFormula365" hidden="1">Formula.SK('[5]NCA Rows'!$A$7,)</definedName>
+    <definedName name="SheetKraftFormula366" hidden="1">Formula.SK('[20]Asset Pivots Grouping'!$G$12,1)</definedName>
+    <definedName name="SheetKraftFormula367" hidden="1">Formula.SK('[20]Asset Pivots Grouping'!$P$4,1)</definedName>
+    <definedName name="SheetKraftFormula368" hidden="1">Formula.SK('[6]Pivots Data'!$R$1,1)</definedName>
+    <definedName name="SheetKraftFormula369" hidden="1">Formula.SK('[6]Pivots Data'!$Q$4,1)</definedName>
+    <definedName name="SheetKraftFormula37" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$X$9,)</definedName>
+    <definedName name="SheetKraftFormula370" hidden="1">Formula.SK('[7]Notes Data'!$GM$10,1)</definedName>
+    <definedName name="SheetKraftFormula371" hidden="1">Formula.SK('[7]Notes Data'!$GT$10,1)</definedName>
+    <definedName name="SheetKraftFormula372" hidden="1">Formula.SK('[7]Notes Data'!$GW$10,1)</definedName>
+    <definedName name="SheetKraftFormula373" hidden="1">Formula.SK('[7]Notes Data'!$HH$10,1)</definedName>
+    <definedName name="SheetKraftFormula374" hidden="1">Formula.SK('[7]Notes Data'!$HM$10,1)</definedName>
+    <definedName name="SheetKraftFormula375" hidden="1">Formula.SK('[7]Notes Data'!$HR$10,1)</definedName>
+    <definedName name="SheetKraftFormula376" hidden="1">Formula.SK('[7]Notes Data'!$HP$10,1)</definedName>
+    <definedName name="SheetKraftFormula377" hidden="1">Formula.SK('[7]Notes Data'!$HQ$11,1)</definedName>
+    <definedName name="SheetKraftFormula378" hidden="1">Formula.SK('[7]Notes Data'!$HW$11,1)</definedName>
+    <definedName name="SheetKraftFormula379" hidden="1">Formula.SK('[13]Rating Master'!$E$8,1)</definedName>
+    <definedName name="SheetKraftFormula38" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$Y$9,)</definedName>
+    <definedName name="SheetKraftFormula380" hidden="1">Formula.SK('[7]Notes Data'!$BT$9,1)</definedName>
+    <definedName name="SheetKraftFormula381" hidden="1">Formula.SK('[7]Notes Data'!$BY$9,1)</definedName>
+    <definedName name="SheetKraftFormula382" hidden="1">Formula.SK('[7]Notes Data'!$BX$9,)</definedName>
+    <definedName name="SheetKraftFormula383" hidden="1">Formula.SK('[7]Notes Data'!$BZ$9,)</definedName>
+    <definedName name="SheetKraftFormula384" hidden="1">Formula.SK('[7]Notes Data'!$CC$9,)</definedName>
+    <definedName name="SheetKraftFormula385" hidden="1">Formula.SK('[7]Notes Data'!$CH$9,1)</definedName>
+    <definedName name="SheetKraftFormula386" hidden="1">Formula.SK('[7]Notes Data'!$CE$10,1)</definedName>
+    <definedName name="SheetKraftFormula387" hidden="1">Formula.SK('[7]Notes Data'!$CG$10,1)</definedName>
+    <definedName name="SheetKraftFormula388" hidden="1">Formula.SK('[7]Notes Data'!$CL$9,1)</definedName>
+    <definedName name="SheetKraftFormula389" hidden="1">Formula.SK('[7]Notes Data'!$CT$9,1)</definedName>
+    <definedName name="SheetKraftFormula39" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$Q$8,)</definedName>
+    <definedName name="SheetKraftFormula390" hidden="1">Formula.SK('[7]Notes Data'!$CV$9,)</definedName>
+    <definedName name="SheetKraftFormula391" hidden="1">Formula.SK('[7]Notes Data'!$CY$9,1)</definedName>
+    <definedName name="SheetKraftFormula392" hidden="1">Formula.SK('[21]No filter Class Master'!$H$11,1)</definedName>
+    <definedName name="SheetKraftFormula393" hidden="1">Formula.SK('[7]Notes Data'!$S$10,1)</definedName>
+    <definedName name="SheetKraftFormula394" hidden="1">Formula.SK('[22]Yes Bank Filter'!$H$9,1)</definedName>
+    <definedName name="SheetKraftFormula395" hidden="1">Formula.SK('[7]Notes Data'!$A$9,1)</definedName>
+    <definedName name="SheetKraftFormula396" hidden="1">Formula.SK('[7]Notes Data'!$T$9,1)</definedName>
+    <definedName name="SheetKraftFormula397" hidden="1">Formula.SK('[7]Notes Data'!$U$9,1)</definedName>
+    <definedName name="SheetKraftFormula398" hidden="1">Formula.SK('[7]Notes Data'!$AT$9,1)</definedName>
+    <definedName name="SheetKraftFormula399" hidden="1">Formula.SK('[7]Notes Data'!$AS$9,)</definedName>
+    <definedName name="SheetKraftFormula4" hidden="1">Formula.SK('[10]Scheme Master'!$B$6,1)</definedName>
+    <definedName name="SheetKraftFormula40" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$AF$14,1)</definedName>
+    <definedName name="SheetKraftFormula401" hidden="1">Formula.SK('[7]Notes Data'!$BA$9,1)</definedName>
+    <definedName name="SheetKraftFormula404" hidden="1">Formula.SK('[7]Notes Data'!$V$10,1)</definedName>
+    <definedName name="SheetKraftFormula405" hidden="1">Formula.SK('[7]Notes Data'!$AZ$10,1)</definedName>
+    <definedName name="SheetKraftFormula406" hidden="1">Formula.SK('[7]Notes Data'!$AR$10,1)</definedName>
+    <definedName name="SheetKraftFormula407" hidden="1">Formula.SK('[23]Notes Data 2'!$F$9,1)</definedName>
+    <definedName name="SheetKraftFormula408" hidden="1">Formula.SK('[23]Notes Data 2'!$M$9,1)</definedName>
+    <definedName name="SheetKraftFormula409" hidden="1">Formula.SK('[23]Notes Data 2'!$E$10,1)</definedName>
+    <definedName name="SheetKraftFormula41" hidden="1">Formula.SK([8]Derivatives!$M$10,1)</definedName>
+    <definedName name="SheetKraftFormula410" hidden="1">Formula.SK('[23]Notes Data 2'!$R$9,1)</definedName>
+    <definedName name="SheetKraftFormula411" hidden="1">Formula.SK('[7]Notes Data'!$K$9,1)</definedName>
+    <definedName name="SheetKraftFormula412" hidden="1">Formula.SK('[24]Avg Yield'!$G$17,1)</definedName>
+    <definedName name="SheetKraftFormula413" hidden="1">Formula.SK('[24]Avg Yield'!$T$17,1)</definedName>
+    <definedName name="SheetKraftFormula414" hidden="1">Formula.SK([2]Stack!$FF$5,1)</definedName>
+    <definedName name="SheetKraftFormula415" hidden="1">Formula.SK([2]Stack!$FG$5,1)</definedName>
+    <definedName name="SheetKraftFormula416" hidden="1">Formula.SK([2]Stack!$FE$6,1)</definedName>
+    <definedName name="SheetKraftFormula417" hidden="1">Formula.SK([2]Stack!$FH$5,1)</definedName>
+    <definedName name="SheetKraftFormula418" hidden="1">Formula.SK([2]Stack!$FL$5,1)</definedName>
+    <definedName name="SheetKraftFormula419" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$J$14,)</definedName>
+    <definedName name="SheetKraftFormula42" hidden="1">Formula.SK([8]Derivatives!$N$11,)</definedName>
+    <definedName name="SheetKraftFormula420" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$I$15,)</definedName>
+    <definedName name="SheetKraftFormula421" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$G$14,)</definedName>
+    <definedName name="SheetKraftFormula422" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$F$14,)</definedName>
+    <definedName name="SheetKraftFormula423" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$H$15,)</definedName>
+    <definedName name="SheetKraftFormula424" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$C$15,)</definedName>
+    <definedName name="SheetKraftFormula425" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$D$15,)</definedName>
+    <definedName name="SheetKraftFormula426" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$E$15,)</definedName>
+    <definedName name="SheetKraftFormula427" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$B$15,)</definedName>
+    <definedName name="SheetKraftFormula428" hidden="1">Formula.SK([2]Stack!$C$5,1)</definedName>
+    <definedName name="SheetKraftFormula429" hidden="1">Formula.SK('[24]Avg Yield'!$Z$17,1)</definedName>
+    <definedName name="SheetKraftFormula43" hidden="1">Formula.SK('[18]Pre Working'!$E$4,1)</definedName>
+    <definedName name="SheetKraftFormula430" hidden="1">Formula.SK('[7]Notes Data'!$EM$22,1)</definedName>
+    <definedName name="SheetKraftFormula431" hidden="1">Formula.SK('[7]Notes Data'!$EN$9,)</definedName>
+    <definedName name="SheetKraftFormula432" hidden="1">Formula.SK('[23]Notes Data 2'!$AE$9,1)</definedName>
+    <definedName name="SheetKraftFormula433" hidden="1">Formula.SK('[23]Notes Data 2'!$AC$9,)</definedName>
+    <definedName name="SheetKraftFormula434" hidden="1">Formula.SK('[23]Notes Data 2'!$AD$9,)</definedName>
+    <definedName name="SheetKraftFormula435" hidden="1">Formula.SK('[23]Notes Data 2'!$AF$9,)</definedName>
+    <definedName name="SheetKraftFormula436" hidden="1">Formula.SK('[23]Notes Data 2'!$AG$9,)</definedName>
+    <definedName name="SheetKraftFormula437" hidden="1">Formula.SK('[23]Notes Data 2'!$AH$9,)</definedName>
+    <definedName name="SheetKraftFormula438" hidden="1">Formula.SK('[23]Notes Data 2'!$AI$9,)</definedName>
+    <definedName name="SheetKraftFormula439" hidden="1">Formula.SK('[23]Notes Data 2'!$AJ$9,)</definedName>
+    <definedName name="SheetKraftFormula44" hidden="1">Formula.SK('[1]Holding Positions'!$R$10,1)</definedName>
+    <definedName name="SheetKraftFormula440" hidden="1">Formula.SK('[23]Notes Data 2'!$AM$9,1)</definedName>
+    <definedName name="SheetKraftFormula441" hidden="1">Formula.SK('[7]Notes Data'!$J$10,1)</definedName>
+    <definedName name="SheetKraftFormula442" hidden="1">Formula.SK('[7]Notes Data'!$H$10,1)</definedName>
+    <definedName name="SheetKraftFormula443" hidden="1">Formula.SK('[26]Liquid Schemes Working Day'!$I$11,)</definedName>
+    <definedName name="SheetKraftFormula444" hidden="1">Formula.SK('[26]Liquid Schemes Working Day'!$J$12,)</definedName>
+    <definedName name="SheetKraftFormula445" hidden="1">Formula.SK('[26]Liquid Schemes Working Day'!$K$12,)</definedName>
+    <definedName name="SheetKraftFormula446" hidden="1">Formula.SK('[26]Liquid Schemes Working Day'!$L$12,)</definedName>
+    <definedName name="SheetKraftFormula447" hidden="1">Formula.SK('[26]Liquid Schemes Working Day'!$P$11,1)</definedName>
+    <definedName name="SheetKraftFormula448" hidden="1">Formula.SK('[26]Liquid Schemes Working Day'!$M$12,1)</definedName>
+    <definedName name="SheetKraftFormula449" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$U$10,)</definedName>
+    <definedName name="SheetKraftFormula45" hidden="1">Formula.SK('[1]Holding Positions'!$S$10,1)</definedName>
+    <definedName name="SheetKraftFormula450" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AI$10,)</definedName>
+    <definedName name="SheetKraftFormula451" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula452" hidden="1">Formula.SK([12]Formats!$G$21,1)</definedName>
+    <definedName name="SheetKraftFormula453" hidden="1">Formula.SK('[27]Riskometer Levels'!$G$18,1)</definedName>
+    <definedName name="SheetKraftFormula454" hidden="1">Formula.SK([2]Stack!$FM$5,1)</definedName>
+    <definedName name="SheetKraftFormula455" hidden="1">Formula.SK('[7]Notes Data'!$GC$9,)</definedName>
+    <definedName name="SheetKraftFormula456" hidden="1">Formula.SK('[7]Notes Data'!$GD$9,)</definedName>
+    <definedName name="SheetKraftFormula457" hidden="1">Formula.SK('[7]Notes Data'!$GB$9,)</definedName>
+    <definedName name="SheetKraftFormula458" hidden="1">Formula.SK('[7]Notes Data'!$GH$9,)</definedName>
+    <definedName name="SheetKraftFormula459" hidden="1">Formula.SK('[7]Notes Data'!$GG$9,)</definedName>
+    <definedName name="SheetKraftFormula460" hidden="1">Formula.SK('[7]Notes Data'!$GI$9,)</definedName>
+    <definedName name="SheetKraftFormula461" hidden="1">Formula.SK('[28]Avg YTC'!$E$13,)</definedName>
+    <definedName name="SheetKraftFormula462" hidden="1">Formula.SK('[28]Avg YTC'!$D$14,1)</definedName>
+    <definedName name="SheetKraftFormula463" hidden="1">Formula.SK([2]Stack!$FN$5,1)</definedName>
+    <definedName name="SheetKraftFormula464" hidden="1">Formula.SK('[22]Yes Bank Filter'!$Q$9,1)</definedName>
+    <definedName name="SheetKraftFormula465" hidden="1">Formula.SK('[22]Yes Bank Filter'!$S$9,1)</definedName>
+    <definedName name="SheetKraftFormula466" hidden="1">Formula.SK('[22]Yes Bank Filter'!$T$9,1)</definedName>
+    <definedName name="SheetKraftFormula467" hidden="1">Formula.SK([2]Stack!$B$5,1)</definedName>
+    <definedName name="SheetKraftFormula468" hidden="1">Formula.SK('[17]Month NAV Last Date Calc'!$AV$7,1)</definedName>
+    <definedName name="SheetKraftFormula469" hidden="1">Formula.SK('[24]Avg Yield'!$AI$13,1)</definedName>
+    <definedName name="SheetKraftFormula470" hidden="1">Formula.SK([2]Stack!$FO$5,1)</definedName>
+    <definedName name="SheetKraftFormula471" hidden="1">Formula.SK('[7]Notes Data'!$IC$10,1)</definedName>
+    <definedName name="SheetKraftFormula472" hidden="1">Formula.SK('[7]Notes Data'!$IB$10,)</definedName>
+    <definedName name="SheetKraftFormula473" hidden="1">Formula.SK('[7]Notes Data'!$IA$10,1)</definedName>
+    <definedName name="SheetKraftFormula474" hidden="1">Formula.SK('[7]Notes Data'!$HZ$10,1)</definedName>
+    <definedName name="SheetKraftFormula475" hidden="1">Formula.SK('[7]Notes Data'!$HY$11,1)</definedName>
+    <definedName name="SheetKraftFormula476" hidden="1">Formula.SK('[7]Notes Data'!$IE$11,1)</definedName>
+    <definedName name="SheetKraftFormula477" hidden="1">Formula.SK('[27]Riskometer Levels'!$L$18,1)</definedName>
+    <definedName name="SheetKraftFormula478" hidden="1">Formula.SK([2]Stack!$FP$5,1)</definedName>
+    <definedName name="SheetKraftFormula479" hidden="1">Formula.SK('[7]Notes Data'!$IF$10,1)</definedName>
+    <definedName name="SheetKraftFormula48" hidden="1">Formula.SK('[1]Holding Positions'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula480" hidden="1">Formula.SK('[7]Notes Data'!$II$10,1)</definedName>
+    <definedName name="SheetKraftFormula481" hidden="1">Formula.SK('[7]Notes Data'!$HC$10,1)</definedName>
+    <definedName name="SheetKraftFormula482" hidden="1">Formula.SK('[7]Notes Data'!$BP$9,1)</definedName>
+    <definedName name="SheetKraftFormula483" hidden="1">Formula.SK('[7]Notes Data'!$BQ$10,1)</definedName>
+    <definedName name="SheetKraftFormula484" hidden="1">Formula.SK('[7]Notes Data'!$BR$10,1)</definedName>
+    <definedName name="SheetKraftFormula486" hidden="1">Formula.SK('[24]Avg Yield'!$AZ$14,1)</definedName>
+    <definedName name="SheetKraftFormula487" hidden="1">Formula.SK([2]Stack!$FQ$5,1)</definedName>
+    <definedName name="SheetKraftFormula488" hidden="1">Formula.SK([8]Derivatives!$U$10,)</definedName>
+    <definedName name="SheetKraftFormula489" hidden="1">Formula.SK([8]Derivatives!$S$10,1)</definedName>
+    <definedName name="SheetKraftFormula490" hidden="1">Formula.SK([8]Derivatives!$R$10,)</definedName>
+    <definedName name="SheetKraftFormula491" hidden="1">Formula.SK([9]Inputs!$N$14,1)</definedName>
+    <definedName name="SheetKraftFormula492" hidden="1">Formula.SK([9]Inputs!$N$6,)</definedName>
+    <definedName name="SheetKraftFormula493" hidden="1">Formula.SK([2]Stack!$FR$6,1)</definedName>
+    <definedName name="SheetKraftFormula494" hidden="1">Formula.SK([2]Stack!$GB$8,1)</definedName>
+    <definedName name="SheetKraftFormula495" hidden="1">Formula.SK([2]Stack!$FS$5,1)</definedName>
+    <definedName name="SheetKraftFormula496" hidden="1">Formula.SK('[7]Notes Data'!$IO$10,1)</definedName>
+    <definedName name="SheetKraftFormula497" hidden="1">Formula.SK('[7]Notes Data'!$IP$10,)</definedName>
+    <definedName name="SheetKraftFormula498" hidden="1">Formula.SK('[29]Foreign Securities'!$E$8,1)</definedName>
+    <definedName name="SheetKraftFormula499" hidden="1">Formula.SK('[29]Foreign Securities'!$J$8,1)</definedName>
+    <definedName name="SheetKraftFormula5" hidden="1">Formula.SK('[1]Holding Positions'!$L$10,1)</definedName>
+    <definedName name="SheetKraftFormula50" hidden="1">Formula.SK('[1]Holding Positions'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula500" hidden="1">Formula.SK('[7]Notes Data'!$DY$9,1)</definedName>
+    <definedName name="SheetKraftFormula501" hidden="1">Formula.SK('[7]Notes Data'!$DX$10,1)</definedName>
+    <definedName name="SheetKraftFormula502" hidden="1">Formula.SK([2]Stack!$BD$5,1)</definedName>
+    <definedName name="SheetKraftFormula503" hidden="1">Formula.SK([2]Stack!$BD$6,1)</definedName>
+    <definedName name="SheetKraftFormula504" hidden="1">Formula.SK('[7]Notes Data'!$CX$9,1)</definedName>
+    <definedName name="SheetKraftFormula506" hidden="1">Formula.SK([2]Stack!$FT$5,1)</definedName>
+    <definedName name="SheetKraftFormula507" hidden="1">Formula.SK([2]Stack!$DG$5,1)</definedName>
+    <definedName name="SheetKraftFormula508" hidden="1">Formula.SK([2]Stack!$GG$8,1)</definedName>
+    <definedName name="SheetKraftFormula509" hidden="1">Formula.SK('[6]Pivots Data'!$CE$4,1)</definedName>
+    <definedName name="SheetKraftFormula51" hidden="1">Formula.SK('[1]Holding Positions'!#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula510" hidden="1">Formula.SK('[30]Management Group'!$B$6,1)</definedName>
+    <definedName name="SheetKraftFormula511" hidden="1">Formula.SK([2]Stack!$FU$5,1)</definedName>
+    <definedName name="SheetKraftFormula512" hidden="1">Formula.SK([2]Stack!$GP$8,1)</definedName>
+    <definedName name="SheetKraftFormula513" hidden="1">Formula.SK('[6]Pivots Data'!$CJ$4,1)</definedName>
+    <definedName name="SheetKraftFormula514" hidden="1">Formula.SK([2]Stack!$GX$8,1)</definedName>
+    <definedName name="SheetKraftFormula515" hidden="1">Formula.SK([2]Stack!$GX$1,1)</definedName>
+    <definedName name="SheetKraftFormula516" hidden="1">Formula.SK('[15]Issuer Master'!$W$10,)</definedName>
+    <definedName name="SheetKraftFormula517" hidden="1">Formula.SK('[25]Perpetual &amp; BT2'!$A$15,1)</definedName>
+    <definedName name="SheetKraftFormula518" hidden="1">Formula.SK([2]Stack!$DD$5,1)</definedName>
+    <definedName name="SheetKraftFormula519" hidden="1">Formula.SK('[7]Notes Data'!$IV$10,)</definedName>
+    <definedName name="SheetKraftFormula52" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula520" hidden="1">Formula.SK('[7]Notes Data'!$IY$11,)</definedName>
+    <definedName name="SheetKraftFormula521" hidden="1">Formula.SK('[7]Notes Data'!$JC$10,)</definedName>
+    <definedName name="SheetKraftFormula522" hidden="1">Formula.SK('[7]Notes Data'!$JF$11,)</definedName>
+    <definedName name="SheetKraftFormula523" hidden="1">Formula.SK('[31]Avg Yield Annualised'!$D$11,1)</definedName>
+    <definedName name="SheetKraftFormula524" hidden="1">Formula.SK([2]Stack!$FV$5,1)</definedName>
+    <definedName name="SheetKraftFormula525" hidden="1">Formula.SK('[16]Security Master'!$Z$9,1)</definedName>
+    <definedName name="SheetKraftFormula527" hidden="1">Formula.SK([8]Derivatives!$O$11,1)</definedName>
+    <definedName name="SheetKraftFormula528" hidden="1">Formula.SK([2]Stack!$FJ$6,1)</definedName>
+    <definedName name="SheetKraftFormula529" hidden="1">Formula.SK([2]Stack!$FK$6,1)</definedName>
+    <definedName name="SheetKraftFormula53" hidden="1">Formula.SK('[1]Holding Positions'!$V$12,1)</definedName>
+    <definedName name="SheetKraftFormula530" hidden="1">Formula.SK('[32]IRS Data'!$E$11,1)</definedName>
+    <definedName name="SheetKraftFormula531" hidden="1">Formula.SK('[32]IRS Data'!$P$11,1)</definedName>
+    <definedName name="SheetKraftFormula532" hidden="1">Formula.SK('[33]Debt Derivative'!$B$5,1)</definedName>
+    <definedName name="SheetKraftFormula533" hidden="1">Formula.SK('[33]Debt Derivative'!$J$5,1)</definedName>
+    <definedName name="SheetKraftFormula534" hidden="1">Formula.SK('[33]Debt Derivative'!$G$5,)</definedName>
+    <definedName name="SheetKraftFormula535" hidden="1">Formula.SK('[33]Debt Derivative'!$P$5,1)</definedName>
+    <definedName name="SheetKraftFormula536" hidden="1">Formula.SK('[33]Debt Derivative'!$W$4,1)</definedName>
+    <definedName name="SheetKraftFormula537" hidden="1">Formula.SK('[33]Debt Derivative'!$AC$5,1)</definedName>
+    <definedName name="SheetKraftFormula538" hidden="1">Formula.SK('[33]Debt Derivative'!$AH$5,1)</definedName>
+    <definedName name="SheetKraftFormula539" hidden="1">Formula.SK('[33]Debt Derivative'!$AG$6,1)</definedName>
+    <definedName name="SheetKraftFormula54" hidden="1">Formula.SK('[1]Holding Positions'!$T$11,1)</definedName>
+    <definedName name="SheetKraftFormula540" hidden="1">Formula.SK('[33]Debt Derivative'!$AF$5,)</definedName>
+    <definedName name="SheetKraftFormula541" hidden="1">Formula.SK('[33]Debt Derivative'!$AO$6,1)</definedName>
+    <definedName name="SheetKraftFormula542" hidden="1">Formula.SK('[33]Debt Derivative'!$AP$6,1)</definedName>
+    <definedName name="SheetKraftFormula543" hidden="1">Formula.SK('[33]Debt Derivative'!$AQ$6,1)</definedName>
+    <definedName name="SheetKraftFormula544" hidden="1">Formula.SK('[33]Debt Derivative'!$AR$6,)</definedName>
+    <definedName name="SheetKraftFormula545" hidden="1">Formula.SK('[33]Debt Derivative'!$AV$13,1)</definedName>
+    <definedName name="SheetKraftFormula546" hidden="1">Formula.SK('[32]IRS Data'!$M$11,1)</definedName>
+    <definedName name="SheetKraftFormula547" hidden="1">Formula.SK('[7]Notes Data'!$EZ$9,1)</definedName>
+    <definedName name="SheetKraftFormula548" hidden="1">Formula.SK('[7]Notes Data'!$EY$9,)</definedName>
+    <definedName name="SheetKraftFormula549" hidden="1">Formula.SK([8]Derivatives!$AW$10,1)</definedName>
+    <definedName name="SheetKraftFormula55" hidden="1">Formula.SK('[18]Pre Working'!$E$5,1)</definedName>
+    <definedName name="SheetKraftFormula550" hidden="1">Formula.SK('[7]Notes Data'!$EW$9,1)</definedName>
+    <definedName name="SheetKraftFormula551" hidden="1">Formula.SK('[7]Notes Data'!$FA$10,1)</definedName>
+    <definedName name="SheetKraftFormula552" hidden="1">Formula.SK('[7]Notes Data'!$FB$9,1)</definedName>
+    <definedName name="SheetKraftFormula553" hidden="1">Formula.SK([8]Derivatives!$T$10,)</definedName>
+    <definedName name="SheetKraftFormula554" hidden="1">Formula.SK('[23]Notes Data 2'!$AY$9,1)</definedName>
+    <definedName name="SheetKraftFormula555" hidden="1">Formula.SK('[23]Notes Data 2'!$AU$9,1)</definedName>
+    <definedName name="SheetKraftFormula556" hidden="1">Formula.SK('[4]Asset Master'!$I$8,1)</definedName>
+    <definedName name="SheetKraftFormula557" hidden="1">Formula.SK('[32]IRS Data'!$Y$11,1)</definedName>
+    <definedName name="SheetKraftFormula558" hidden="1">Formula.SK('[32]IRS Data'!$X$11,1)</definedName>
+    <definedName name="SheetKraftFormula559" hidden="1">Formula.SK('[32]IRS Data'!$U$11,1)</definedName>
+    <definedName name="SheetKraftFormula560" hidden="1">Formula.SK('[20]Asset Pivots Grouping'!$O$13,1)</definedName>
+    <definedName name="SheetKraftFormula561" hidden="1">Formula.SK('[20]Asset Pivots Grouping'!$P$13,)</definedName>
+    <definedName name="SheetKraftFormula562" hidden="1">Formula.SK('[6]Pivots Data'!$BC$5,1)</definedName>
+    <definedName name="SheetKraftFormula563" hidden="1">Formula.SK([9]Inputs!$AG$3,1)</definedName>
+    <definedName name="SheetKraftFormula564" hidden="1">Formula.SK([9]Inputs!$AJ$3,1)</definedName>
+    <definedName name="SheetKraftFormula565" hidden="1">Formula.SK('[7]Notes Data'!$X$10,1)</definedName>
+    <definedName name="SheetKraftFormula566" hidden="1">Formula.SK('[23]Notes Data 2'!$AV$10,1)</definedName>
+    <definedName name="SheetKraftFormula567" hidden="1">Formula.SK('[26]Liquid Schemes Working Day'!$N$12,1)</definedName>
+    <definedName name="SheetKraftFormula57" hidden="1">Formula.SK('[18]Pre Working'!$K$5,1)</definedName>
+    <definedName name="SheetKraftFormula58" hidden="1">Formula.SK('[7]Notes Data'!$B$9,1)</definedName>
+    <definedName name="SheetKraftFormula59" hidden="1">Formula.SK('[7]Notes Data'!$Z$9,1)</definedName>
+    <definedName name="SheetKraftFormula6" hidden="1">Formula.SK('[16]Security Master'!$C$8,1)</definedName>
+    <definedName name="SheetKraftFormula61" hidden="1">Formula.SK('[18]Pre Working'!$AC$5,1)</definedName>
+    <definedName name="SheetKraftFormula62" hidden="1">Formula.SK('[18]Pre Working'!$AL$5,1)</definedName>
+    <definedName name="SheetKraftFormula63" hidden="1">Formula.SK('[16]Security Master'!$X$8,1)</definedName>
+    <definedName name="SheetKraftFormula64" hidden="1">Formula.SK('[4]Asset Master'!$T$7,1)</definedName>
+    <definedName name="SheetKraftFormula65" hidden="1">Formula.SK('[4]Asset Master'!$P$6,1)</definedName>
+    <definedName name="SheetKraftFormula66" hidden="1">Formula.SK('[18]Pre Working'!$AN$5,1)</definedName>
+    <definedName name="SheetKraftFormula67" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$Z$8,1)</definedName>
+    <definedName name="SheetKraftFormula68" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula69" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula7" hidden="1">Formula.SK('[16]Security Master'!$U$9,1)</definedName>
+    <definedName name="SheetKraftFormula70" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula71" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula72" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula73" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula74" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula75" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula76" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula77" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula78" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula79" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula8" hidden="1">Formula.SK('[16]Security Master'!$V$9,1)</definedName>
+    <definedName name="SheetKraftFormula80" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula81" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula82" hidden="1">Formula.SK(#REF!,)</definedName>
+    <definedName name="SheetKraftFormula83" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula84" hidden="1">Formula.SK(#REF!,1)</definedName>
+    <definedName name="SheetKraftFormula85" hidden="1">Formula.SK('[5]NCA Rows'!$D$4,1)</definedName>
+    <definedName name="SheetKraftFormula86" hidden="1">Formula.SK('[14]NCA Calc, Repo'!$Z$9,1)</definedName>
+    <definedName name="SheetKraftFormula87" hidden="1">Formula.SK('[5]NCA Rows'!$H$4,1)</definedName>
+    <definedName name="SheetKraftFormula88" hidden="1">Formula.SK('[5]NCA Rows'!$AJ$4,)</definedName>
+    <definedName name="SheetKraftFormula89" hidden="1">Formula.SK('[5]NCA Rows'!$AK$4,)</definedName>
+    <definedName name="SheetKraftFormula9" hidden="1">Formula.SK('[16]Security Master'!$W$9,1)</definedName>
+    <definedName name="SheetKraftFormula90" hidden="1">Formula.SK('[5]NCA Rows'!$AM$4,1)</definedName>
+    <definedName name="SheetKraftFormula91" hidden="1">Formula.SK('[5]NCA Rows'!$C$4,)</definedName>
+    <definedName name="SheetKraftFormula92" hidden="1">Formula.SK('[5]NCA Rows'!$J$4,)</definedName>
+    <definedName name="SheetKraftFormula93" hidden="1">Formula.SK('[5]NCA Rows'!$E$4,1)</definedName>
+    <definedName name="SheetKraftFormula95" hidden="1">Formula.SK('[5]NCA Rows'!$N$4,)</definedName>
+    <definedName name="SheetKraftFormula96" hidden="1">Formula.SK('[5]NCA Rows'!$AN$4,)</definedName>
+    <definedName name="SheetKraftFormula98" hidden="1">Formula.SK([2]Stack!$E$4,1)</definedName>
+    <definedName name="SheetKraftFormula99" hidden="1">Formula.SK([2]Stack!$AT$5,1)</definedName>
     <definedName name="SheetKraftInput1" hidden="1">INDEX([9]Inputs!$B$1,,)</definedName>
     <definedName name="SheetKraftInput2" hidden="1">INDEX([9]Inputs!$F$2,,)</definedName>
     <definedName name="SheetKraftOutput1" hidden="1">INDEX([3]Template_Formula!$A$3,,)</definedName>
@@ -595,7 +590,7 @@
     <definedName name="SheetKraftOutput4" hidden="1">INDEX('[7]Notes Data'!$II$9,,)</definedName>
     <definedName name="SheetKraftOutput5" hidden="1">INDEX([2]Stack!$GX$7,,)</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1345,12 +1340,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1594,7 +1589,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-3500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-3500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1606,7 +1601,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" r:link="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1644,7 +1639,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-3500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-3500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1656,7 +1651,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" r:link="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1680,7 +1675,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Holding Positions"/>
@@ -1693,7 +1688,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Scheme Master"/>
@@ -1706,7 +1701,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Scheme Category"/>
@@ -1719,7 +1714,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Formats"/>
@@ -1732,7 +1727,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Rating Master"/>
@@ -1745,7 +1740,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="NCA Calc, Repo"/>
@@ -1758,7 +1753,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Issuer Master"/>
@@ -1771,7 +1766,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Security Master"/>
@@ -1784,7 +1779,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Month NAV Last Date Calc"/>
@@ -1797,7 +1792,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Pre Working"/>
@@ -1810,7 +1805,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Repo Rows"/>
@@ -1823,7 +1818,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Stack"/>
@@ -1836,7 +1831,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Asset Pivots Grouping"/>
@@ -1849,7 +1844,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="No filter Class Master"/>
@@ -1862,7 +1857,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink22.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Yes Bank Filter"/>
@@ -1875,7 +1870,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink23.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Notes Data 2"/>
@@ -1888,7 +1883,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Avg Yield"/>
@@ -1901,7 +1896,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Perpetual &amp; BT2"/>
@@ -1914,7 +1909,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Liquid Schemes Working Day"/>
@@ -1927,7 +1922,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Riskometer Levels"/>
@@ -1940,7 +1935,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Avg YTC"/>
@@ -1953,7 +1948,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Foreign Securities"/>
@@ -1966,7 +1961,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Template_Formula"/>
@@ -1979,7 +1974,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink30.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Management Group"/>
@@ -1992,7 +1987,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Avg Yield Annualised"/>
@@ -2005,7 +2000,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink32.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="IRS Data"/>
@@ -2018,7 +2013,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink33.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Debt Derivative"/>
@@ -2031,7 +2026,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Asset Master"/>
@@ -2044,7 +2039,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="NCA Rows"/>
@@ -2057,7 +2052,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Pivots Data"/>
@@ -2070,7 +2065,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Notes Data"/>
@@ -2083,7 +2078,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Derivatives"/>
@@ -2096,7 +2091,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Inputs"/>
@@ -2151,7 +2146,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2186,7 +2181,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2363,22 +2358,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet54"/>
   <dimension ref="A1:L183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G200" sqref="G200"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" style="3" customWidth="1"/>
@@ -2393,7 +2388,7 @@
     <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="46.5" customHeight="1">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -2431,7 +2426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="34" t="s">
         <v>3</v>
       </c>
@@ -2465,7 +2460,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -2477,7 +2472,7 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2491,7 +2486,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="26.25">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>4</v>
@@ -2527,7 +2522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
         <v>14</v>
@@ -2543,7 +2538,7 @@
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
         <v>15</v>
@@ -2559,7 +2554,7 @@
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
         <v>16</v>
@@ -2575,7 +2570,7 @@
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
@@ -2613,7 +2608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
@@ -2651,7 +2646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
@@ -2689,7 +2684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -2727,7 +2722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
@@ -2765,7 +2760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
@@ -2803,7 +2798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="10" t="s">
         <v>17</v>
       </c>
@@ -2841,7 +2836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
@@ -2879,7 +2874,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="10" t="s">
         <v>17</v>
       </c>
@@ -2917,7 +2912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="10" t="s">
         <v>17</v>
       </c>
@@ -2955,7 +2950,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="10" t="s">
         <v>13</v>
       </c>
@@ -2993,7 +2988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="10" t="s">
         <v>13</v>
       </c>
@@ -3031,7 +3026,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="10" t="s">
         <v>13</v>
       </c>
@@ -3069,7 +3064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="10" t="s">
         <v>13</v>
       </c>
@@ -3107,7 +3102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="10" t="s">
         <v>13</v>
       </c>
@@ -3145,7 +3140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="10" t="s">
         <v>13</v>
       </c>
@@ -3183,7 +3178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="10" t="s">
         <v>13</v>
       </c>
@@ -3221,7 +3216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="10" t="s">
         <v>13</v>
       </c>
@@ -3259,7 +3254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="10" t="s">
         <v>13</v>
       </c>
@@ -3297,7 +3292,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="10" t="s">
         <v>13</v>
       </c>
@@ -3335,7 +3330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="10" t="s">
         <v>13</v>
       </c>
@@ -3373,7 +3368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="10" t="s">
         <v>13</v>
       </c>
@@ -3411,7 +3406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="10" t="s">
         <v>13</v>
       </c>
@@ -3449,7 +3444,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="10" t="s">
         <v>13</v>
       </c>
@@ -3487,7 +3482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="10" t="s">
         <v>13</v>
       </c>
@@ -3525,7 +3520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="10" t="s">
         <v>13</v>
       </c>
@@ -3563,7 +3558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="10" t="s">
         <v>13</v>
       </c>
@@ -3601,7 +3596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="10" t="s">
         <v>13</v>
       </c>
@@ -3639,7 +3634,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="10" t="s">
         <v>13</v>
       </c>
@@ -3677,7 +3672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="10" t="s">
         <v>13</v>
       </c>
@@ -3715,7 +3710,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="10" t="s">
         <v>13</v>
       </c>
@@ -3753,7 +3748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="10" t="s">
         <v>13</v>
       </c>
@@ -3791,7 +3786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="10" t="s">
         <v>13</v>
       </c>
@@ -3829,7 +3824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="10" t="s">
         <v>13</v>
       </c>
@@ -3867,7 +3862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="10" t="s">
         <v>13</v>
       </c>
@@ -3905,7 +3900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" s="10" t="s">
         <v>13</v>
       </c>
@@ -3943,7 +3938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" s="10" t="s">
         <v>13</v>
       </c>
@@ -3981,7 +3976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46" s="10" t="s">
         <v>13</v>
       </c>
@@ -4019,7 +4014,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47" s="10" t="s">
         <v>13</v>
       </c>
@@ -4057,7 +4052,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" s="10" t="s">
         <v>13</v>
       </c>
@@ -4095,7 +4090,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" s="10" t="s">
         <v>13</v>
       </c>
@@ -4133,7 +4128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50" s="10" t="s">
         <v>13</v>
       </c>
@@ -4171,7 +4166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51" s="10" t="s">
         <v>13</v>
       </c>
@@ -4209,7 +4204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52" s="10" t="s">
         <v>13</v>
       </c>
@@ -4247,7 +4242,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" s="10" t="s">
         <v>13</v>
       </c>
@@ -4285,7 +4280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" s="10" t="s">
         <v>13</v>
       </c>
@@ -4323,7 +4318,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" s="10" t="s">
         <v>13</v>
       </c>
@@ -4361,7 +4356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56" s="10" t="s">
         <v>13</v>
       </c>
@@ -4399,7 +4394,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57" s="10" t="s">
         <v>13</v>
       </c>
@@ -4437,7 +4432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58" s="10" t="s">
         <v>13</v>
       </c>
@@ -4475,7 +4470,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59" s="10" t="s">
         <v>13</v>
       </c>
@@ -4513,7 +4508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60" s="10" t="s">
         <v>13</v>
       </c>
@@ -4551,7 +4546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61" s="10" t="s">
         <v>13</v>
       </c>
@@ -4589,7 +4584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62" s="10" t="s">
         <v>13</v>
       </c>
@@ -4627,7 +4622,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63" s="10" t="s">
         <v>13</v>
       </c>
@@ -4665,7 +4660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="A64" s="10" t="s">
         <v>13</v>
       </c>
@@ -4703,7 +4698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12">
       <c r="A65" s="10" t="s">
         <v>13</v>
       </c>
@@ -4741,7 +4736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12">
       <c r="A66" s="10" t="s">
         <v>13</v>
       </c>
@@ -4779,7 +4774,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="A67" s="10" t="s">
         <v>13</v>
       </c>
@@ -4817,7 +4812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12">
       <c r="A68" s="10" t="s">
         <v>13</v>
       </c>
@@ -4855,7 +4850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12">
       <c r="A69" s="10" t="s">
         <v>13</v>
       </c>
@@ -4893,7 +4888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12">
       <c r="A70" s="10" t="s">
         <v>13</v>
       </c>
@@ -4931,7 +4926,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12">
       <c r="A71" s="10" t="s">
         <v>13</v>
       </c>
@@ -4969,7 +4964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12">
       <c r="A72" s="10" t="s">
         <v>13</v>
       </c>
@@ -5007,7 +5002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12">
       <c r="A73" s="10" t="s">
         <v>13</v>
       </c>
@@ -5045,7 +5040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12">
       <c r="A74" s="10" t="s">
         <v>13</v>
       </c>
@@ -5083,7 +5078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12">
       <c r="A75" s="10" t="s">
         <v>13</v>
       </c>
@@ -5121,7 +5116,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12">
       <c r="A76" s="10" t="s">
         <v>13</v>
       </c>
@@ -5159,7 +5154,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12">
       <c r="A77" s="10" t="s">
         <v>13</v>
       </c>
@@ -5197,7 +5192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12">
       <c r="A78" s="10" t="s">
         <v>13</v>
       </c>
@@ -5235,7 +5230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12">
       <c r="A79" s="10" t="s">
         <v>13</v>
       </c>
@@ -5273,7 +5268,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12">
       <c r="A80" s="10" t="s">
         <v>13</v>
       </c>
@@ -5311,7 +5306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12">
       <c r="A81" s="10" t="s">
         <v>13</v>
       </c>
@@ -5349,7 +5344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12">
       <c r="A82" s="10" t="s">
         <v>13</v>
       </c>
@@ -5387,7 +5382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12">
       <c r="A83" s="10" t="s">
         <v>13</v>
       </c>
@@ -5425,7 +5420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12">
       <c r="A84" s="10" t="s">
         <v>13</v>
       </c>
@@ -5463,7 +5458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12">
       <c r="A85" s="10" t="s">
         <v>13</v>
       </c>
@@ -5501,7 +5496,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12">
       <c r="A86" s="10" t="s">
         <v>13</v>
       </c>
@@ -5539,7 +5534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12">
       <c r="A87" s="10" t="s">
         <v>13</v>
       </c>
@@ -5577,7 +5572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12">
       <c r="A88" s="17"/>
       <c r="B88" s="9" t="s">
         <v>207</v>
@@ -5597,7 +5592,7 @@
       <c r="K88" s="17"/>
       <c r="L88" s="17"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12">
       <c r="A89" s="8"/>
       <c r="B89" s="9" t="s">
         <v>208</v>
@@ -5617,7 +5612,7 @@
       <c r="K89" s="8"/>
       <c r="L89" s="8"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12">
       <c r="A90" s="8"/>
       <c r="B90" s="9" t="s">
         <v>209</v>
@@ -5633,7 +5628,7 @@
       <c r="K90" s="8"/>
       <c r="L90" s="8"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12">
       <c r="A91" s="8"/>
       <c r="B91" s="9" t="s">
         <v>210</v>
@@ -5649,7 +5644,7 @@
       <c r="K91" s="8"/>
       <c r="L91" s="8"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12">
       <c r="A92" s="10" t="s">
         <v>13</v>
       </c>
@@ -5687,7 +5682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12">
       <c r="A93" s="17"/>
       <c r="B93" s="9" t="s">
         <v>207</v>
@@ -5707,7 +5702,7 @@
       <c r="K93" s="17"/>
       <c r="L93" s="17"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12">
       <c r="A94" s="8"/>
       <c r="B94" s="9" t="s">
         <v>208</v>
@@ -5727,7 +5722,7 @@
       <c r="K94" s="8"/>
       <c r="L94" s="8"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12">
       <c r="A95" s="8"/>
       <c r="B95" s="9" t="s">
         <v>211</v>
@@ -5743,7 +5738,7 @@
       <c r="K95" s="8"/>
       <c r="L95" s="8"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12">
       <c r="A96" s="8"/>
       <c r="B96" s="9" t="s">
         <v>212</v>
@@ -5759,7 +5754,7 @@
       <c r="K96" s="8"/>
       <c r="L96" s="8"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12">
       <c r="A97" s="10" t="s">
         <v>13</v>
       </c>
@@ -5797,7 +5792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12">
       <c r="A98" s="17"/>
       <c r="B98" s="9" t="s">
         <v>207</v>
@@ -5817,7 +5812,7 @@
       <c r="K98" s="17"/>
       <c r="L98" s="17"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12">
       <c r="A99" s="8"/>
       <c r="B99" s="9" t="s">
         <v>208</v>
@@ -5837,7 +5832,7 @@
       <c r="K99" s="8"/>
       <c r="L99" s="8"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -5851,7 +5846,7 @@
       <c r="K100" s="4"/>
       <c r="L100" s="4"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12">
       <c r="A101" s="4"/>
       <c r="B101" s="20" t="s">
         <v>213</v>
@@ -5871,7 +5866,7 @@
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12">
       <c r="A102" s="10" t="s">
         <v>17</v>
       </c>
@@ -5897,7 +5892,7 @@
       <c r="K102" s="11"/>
       <c r="L102" s="11"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12">
       <c r="A103" s="11"/>
       <c r="B103" s="32" t="s">
         <v>215</v>
@@ -5921,7 +5916,7 @@
       <c r="K103" s="11"/>
       <c r="L103" s="11"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12">
       <c r="A104" s="11"/>
       <c r="B104" s="32" t="s">
         <v>216</v>
@@ -5945,7 +5940,7 @@
       <c r="K104" s="11"/>
       <c r="L104" s="11"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12">
       <c r="A105" s="11"/>
       <c r="B105" s="32" t="s">
         <v>217</v>
@@ -5969,7 +5964,7 @@
       <c r="K105" s="11"/>
       <c r="L105" s="11"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12">
       <c r="A106" s="11"/>
       <c r="B106" s="32" t="s">
         <v>218</v>
@@ -5993,7 +5988,7 @@
       <c r="K106" s="11"/>
       <c r="L106" s="11"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12">
       <c r="A107" s="11"/>
       <c r="B107" s="32" t="s">
         <v>219</v>
@@ -6017,7 +6012,7 @@
       <c r="K107" s="11"/>
       <c r="L107" s="11"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12">
       <c r="A108" s="11"/>
       <c r="B108" s="32" t="s">
         <v>220</v>
@@ -6041,7 +6036,7 @@
       <c r="K108" s="11"/>
       <c r="L108" s="11"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12">
       <c r="A109" s="11"/>
       <c r="B109" s="32" t="s">
         <v>221</v>
@@ -6065,7 +6060,7 @@
       <c r="K109" s="11"/>
       <c r="L109" s="11"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12">
       <c r="A110" s="11"/>
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
@@ -6075,7 +6070,7 @@
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12">
       <c r="A111" s="22"/>
       <c r="B111" s="23" t="s">
         <v>222</v>
@@ -6087,7 +6082,7 @@
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12">
       <c r="A112" s="22"/>
       <c r="B112" s="24" t="s">
         <v>23</v>
@@ -6101,7 +6096,7 @@
       <c r="G112" s="11"/>
       <c r="H112" s="11"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8">
       <c r="A113" s="22"/>
       <c r="B113" s="24" t="s">
         <v>26</v>
@@ -6115,7 +6110,7 @@
       <c r="G113" s="11"/>
       <c r="H113" s="11"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8">
       <c r="A114" s="22"/>
       <c r="B114" s="24" t="s">
         <v>35</v>
@@ -6129,7 +6124,7 @@
       <c r="G114" s="11"/>
       <c r="H114" s="11"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8">
       <c r="A115" s="22"/>
       <c r="B115" s="24" t="s">
         <v>32</v>
@@ -6143,7 +6138,7 @@
       <c r="G115" s="11"/>
       <c r="H115" s="11"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8">
       <c r="A116" s="22"/>
       <c r="B116" s="24" t="s">
         <v>76</v>
@@ -6157,7 +6152,7 @@
       <c r="G116" s="11"/>
       <c r="H116" s="11"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8">
       <c r="A117" s="22"/>
       <c r="B117" s="24" t="s">
         <v>20</v>
@@ -6171,7 +6166,7 @@
       <c r="G117" s="11"/>
       <c r="H117" s="11"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8">
       <c r="A118" s="22"/>
       <c r="B118" s="24" t="s">
         <v>79</v>
@@ -6185,7 +6180,7 @@
       <c r="G118" s="11"/>
       <c r="H118" s="11"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8">
       <c r="A119" s="22"/>
       <c r="B119" s="24" t="s">
         <v>60</v>
@@ -6199,7 +6194,7 @@
       <c r="G119" s="11"/>
       <c r="H119" s="11"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8">
       <c r="A120" s="22"/>
       <c r="B120" s="24" t="s">
         <v>29</v>
@@ -6213,7 +6208,7 @@
       <c r="G120" s="11"/>
       <c r="H120" s="11"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8">
       <c r="A121" s="22"/>
       <c r="B121" s="24" t="s">
         <v>52</v>
@@ -6227,7 +6222,7 @@
       <c r="G121" s="11"/>
       <c r="H121" s="11"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8">
       <c r="A122" s="22"/>
       <c r="B122" s="24" t="s">
         <v>38</v>
@@ -6241,7 +6236,7 @@
       <c r="G122" s="11"/>
       <c r="H122" s="11"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8">
       <c r="A123" s="22"/>
       <c r="B123" s="24" t="s">
         <v>73</v>
@@ -6255,7 +6250,7 @@
       <c r="G123" s="11"/>
       <c r="H123" s="11"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8">
       <c r="A124" s="22"/>
       <c r="B124" s="24" t="s">
         <v>49</v>
@@ -6269,7 +6264,7 @@
       <c r="G124" s="11"/>
       <c r="H124" s="11"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8">
       <c r="A125" s="22"/>
       <c r="B125" s="24" t="s">
         <v>101</v>
@@ -6283,7 +6278,7 @@
       <c r="G125" s="11"/>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8">
       <c r="A126" s="22"/>
       <c r="B126" s="24" t="s">
         <v>57</v>
@@ -6297,7 +6292,7 @@
       <c r="G126" s="11"/>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8">
       <c r="A127" s="22"/>
       <c r="B127" s="24" t="s">
         <v>129</v>
@@ -6311,7 +6306,7 @@
       <c r="G127" s="11"/>
       <c r="H127" s="11"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8">
       <c r="A128" s="22"/>
       <c r="B128" s="24" t="s">
         <v>63</v>
@@ -6325,7 +6320,7 @@
       <c r="G128" s="11"/>
       <c r="H128" s="11"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8">
       <c r="A129" s="22"/>
       <c r="B129" s="24" t="s">
         <v>70</v>
@@ -6339,7 +6334,7 @@
       <c r="G129" s="11"/>
       <c r="H129" s="11"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8">
       <c r="A130" s="22"/>
       <c r="B130" s="24" t="s">
         <v>126</v>
@@ -6353,7 +6348,7 @@
       <c r="G130" s="11"/>
       <c r="H130" s="11"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8">
       <c r="A131" s="22"/>
       <c r="B131" s="24" t="s">
         <v>82</v>
@@ -6367,7 +6362,7 @@
       <c r="G131" s="11"/>
       <c r="H131" s="11"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8">
       <c r="A132" s="22"/>
       <c r="B132" s="24" t="s">
         <v>91</v>
@@ -6381,7 +6376,7 @@
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8">
       <c r="A133" s="22"/>
       <c r="B133" s="24" t="s">
         <v>96</v>
@@ -6395,7 +6390,7 @@
       <c r="G133" s="11"/>
       <c r="H133" s="11"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8">
       <c r="A134" s="22"/>
       <c r="B134" s="24" t="s">
         <v>104</v>
@@ -6409,7 +6404,7 @@
       <c r="G134" s="11"/>
       <c r="H134" s="11"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8">
       <c r="A135" s="22"/>
       <c r="B135" s="24" t="s">
         <v>139</v>
@@ -6423,7 +6418,7 @@
       <c r="G135" s="11"/>
       <c r="H135" s="11"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8">
       <c r="A136" s="22"/>
       <c r="B136" s="24" t="s">
         <v>123</v>
@@ -6437,7 +6432,7 @@
       <c r="G136" s="11"/>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8">
       <c r="A137" s="22"/>
       <c r="B137" s="24" t="s">
         <v>173</v>
@@ -6451,7 +6446,7 @@
       <c r="G137" s="11"/>
       <c r="H137" s="11"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8">
       <c r="A138" s="22"/>
       <c r="B138" s="24" t="s">
         <v>134</v>
@@ -6465,7 +6460,7 @@
       <c r="G138" s="11"/>
       <c r="H138" s="11"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8">
       <c r="A139" s="22"/>
       <c r="B139" s="24" t="s">
         <v>160</v>
@@ -6479,7 +6474,7 @@
       <c r="G139" s="11"/>
       <c r="H139" s="11"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8">
       <c r="A140" s="22"/>
       <c r="B140" s="24" t="s">
         <v>186</v>
@@ -6493,7 +6488,7 @@
       <c r="G140" s="11"/>
       <c r="H140" s="11"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8">
       <c r="A141" s="22"/>
       <c r="B141" s="24" t="s">
         <v>201</v>
@@ -6507,7 +6502,7 @@
       <c r="G141" s="11"/>
       <c r="H141" s="11"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8">
       <c r="A142" s="22"/>
       <c r="B142" s="24" t="s">
         <v>206</v>
@@ -6521,7 +6516,7 @@
       <c r="G142" s="11"/>
       <c r="H142" s="11"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8">
       <c r="A143" s="22"/>
       <c r="B143" s="24" t="s">
         <v>223</v>
@@ -6535,7 +6530,7 @@
       <c r="G143" s="11"/>
       <c r="H143" s="11"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8">
       <c r="A144" s="27"/>
       <c r="B144" s="27"/>
       <c r="C144" s="27"/>
@@ -6545,7 +6540,7 @@
       <c r="G144" s="27"/>
       <c r="H144" s="27"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8">
       <c r="A145" s="27"/>
       <c r="B145" s="8" t="s">
         <v>224</v>
@@ -6557,7 +6552,7 @@
       <c r="G145" s="27"/>
       <c r="H145" s="27"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8">
       <c r="A146" s="11"/>
       <c r="B146" s="11" t="s">
         <v>225</v>
@@ -6569,7 +6564,7 @@
       <c r="G146" s="11"/>
       <c r="H146" s="27"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8">
       <c r="A147" s="11"/>
       <c r="B147" s="28" t="s">
         <v>226</v>
@@ -6585,7 +6580,7 @@
       <c r="G147" s="11"/>
       <c r="H147" s="27"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8">
       <c r="A148" s="11"/>
       <c r="B148" s="8" t="s">
         <v>229</v>
@@ -6601,7 +6596,7 @@
       <c r="G148" s="11"/>
       <c r="H148" s="27"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8">
       <c r="A149" s="11"/>
       <c r="B149" s="8" t="s">
         <v>230</v>
@@ -6617,7 +6612,7 @@
       <c r="G149" s="11"/>
       <c r="H149" s="27"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8">
       <c r="A150" s="11"/>
       <c r="B150" s="8" t="s">
         <v>231</v>
@@ -6633,7 +6628,7 @@
       <c r="G150" s="11"/>
       <c r="H150" s="27"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8">
       <c r="A151" s="11"/>
       <c r="B151" s="8" t="s">
         <v>232</v>
@@ -6649,7 +6644,7 @@
       <c r="G151" s="11"/>
       <c r="H151" s="27"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8">
       <c r="A152" s="11"/>
       <c r="B152" s="8" t="s">
         <v>13</v>
@@ -6661,7 +6656,7 @@
       <c r="G152" s="11"/>
       <c r="H152" s="27"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8">
       <c r="A153" s="11"/>
       <c r="B153" s="11"/>
       <c r="C153" s="11"/>
@@ -6671,7 +6666,7 @@
       <c r="G153" s="11"/>
       <c r="H153" s="27"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8">
       <c r="A154" s="11"/>
       <c r="B154" s="11" t="s">
         <v>233</v>
@@ -6683,7 +6678,7 @@
       <c r="G154" s="11"/>
       <c r="H154" s="27"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8">
       <c r="A155" s="11"/>
       <c r="B155" s="11"/>
       <c r="C155" s="11"/>
@@ -6693,7 +6688,7 @@
       <c r="G155" s="11"/>
       <c r="H155" s="27"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8">
       <c r="A156" s="11"/>
       <c r="B156" s="11" t="s">
         <v>234</v>
@@ -6705,7 +6700,7 @@
       <c r="G156" s="11"/>
       <c r="H156" s="27"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8">
       <c r="A157" s="27"/>
       <c r="B157" s="27"/>
       <c r="C157" s="27"/>
@@ -6715,7 +6710,7 @@
       <c r="G157" s="27"/>
       <c r="H157" s="27"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8">
       <c r="A158" s="11"/>
       <c r="B158" s="11" t="s">
         <v>235</v>
@@ -6727,7 +6722,7 @@
       <c r="G158" s="11"/>
       <c r="H158" s="11"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8">
       <c r="A159" s="11"/>
       <c r="B159" s="11" t="s">
         <v>236</v>
@@ -6739,7 +6734,7 @@
       <c r="G159" s="11"/>
       <c r="H159" s="27"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8">
       <c r="A160" s="11"/>
       <c r="B160" s="11" t="s">
         <v>237</v>
@@ -6751,7 +6746,7 @@
       <c r="G160" s="11"/>
       <c r="H160" s="27"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8">
       <c r="A161" s="11"/>
       <c r="B161" s="11" t="s">
         <v>238</v>
@@ -6763,7 +6758,7 @@
       <c r="G161" s="11"/>
       <c r="H161" s="27"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8">
       <c r="A162" s="11"/>
       <c r="B162" s="11" t="s">
         <v>239</v>
@@ -6775,7 +6770,7 @@
       <c r="G162" s="11"/>
       <c r="H162" s="27"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8">
       <c r="A163" s="11"/>
       <c r="B163" s="11" t="s">
         <v>240</v>
@@ -6787,7 +6782,7 @@
       <c r="G163" s="11"/>
       <c r="H163" s="27"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8">
       <c r="A164" s="11"/>
       <c r="B164" s="11" t="s">
         <v>241</v>
@@ -6799,7 +6794,7 @@
       <c r="G164" s="11"/>
       <c r="H164" s="27"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8">
       <c r="A165" s="11"/>
       <c r="B165" s="11" t="s">
         <v>242</v>
@@ -6811,12 +6806,12 @@
       <c r="G165" s="11"/>
       <c r="H165" s="27"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8">
       <c r="B167" s="31" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2">
       <c r="B183" s="31" t="s">
         <v>244</v>
       </c>

</xml_diff>